<commit_message>
Añadida la semana 2
</commit_message>
<xml_diff>
--- a/LEC.xlsx
+++ b/LEC.xlsx
@@ -882,13 +882,13 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:AC705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1289,26 +1289,26 @@
       <c r="Z2" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="AA2" s="31"/>
+      <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="5:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J3" s="37"/>
       <c r="K3" s="38"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="32"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="31"/>
       <c r="AA3" s="34"/>
     </row>
     <row r="4" spans="5:28" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1407,8 +1407,12 @@
       <c r="K5" s="9">
         <v>7</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
+      <c r="L5" s="9">
+        <v>19</v>
+      </c>
+      <c r="M5" s="9">
+        <v>4</v>
+      </c>
       <c r="N5" s="9">
         <v>13</v>
       </c>
@@ -1429,7 +1433,7 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9">
         <f>SUM(J5:AA5)</f>
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1454,8 +1458,12 @@
       <c r="K6" s="9">
         <v>9</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="L6" s="9">
+        <v>20</v>
+      </c>
+      <c r="M6" s="9">
+        <v>7</v>
+      </c>
       <c r="N6" s="9">
         <v>10</v>
       </c>
@@ -1476,7 +1484,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9">
         <f t="shared" ref="AB6:AB69" si="0">SUM(J6:AA6)</f>
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1501,8 +1509,12 @@
       <c r="K7" s="9">
         <v>11</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="L7" s="9">
+        <v>23</v>
+      </c>
+      <c r="M7" s="9">
+        <v>10</v>
+      </c>
       <c r="N7" s="9">
         <v>13</v>
       </c>
@@ -1523,7 +1535,7 @@
       <c r="AA7" s="9"/>
       <c r="AB7" s="9">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1548,8 +1560,12 @@
       <c r="K8" s="9">
         <v>13</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
+      <c r="L8" s="9">
+        <v>27</v>
+      </c>
+      <c r="M8" s="9">
+        <v>10</v>
+      </c>
       <c r="N8" s="9">
         <v>9</v>
       </c>
@@ -1570,7 +1586,7 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1595,8 +1611,12 @@
       <c r="K9" s="9">
         <v>11</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="L9" s="9">
+        <v>26</v>
+      </c>
+      <c r="M9" s="9">
+        <v>1</v>
+      </c>
       <c r="N9" s="9">
         <v>11</v>
       </c>
@@ -1617,7 +1637,7 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1912,8 +1932,12 @@
       <c r="K16" s="9">
         <v>13</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="L16" s="9">
+        <v>31</v>
+      </c>
+      <c r="M16" s="9">
+        <v>19</v>
+      </c>
       <c r="N16" s="9">
         <v>11</v>
       </c>
@@ -1934,7 +1958,7 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1988,8 +2012,12 @@
       <c r="K18" s="9">
         <v>14</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="L18" s="9">
+        <v>10</v>
+      </c>
+      <c r="M18" s="9">
+        <v>12</v>
+      </c>
       <c r="N18" s="9">
         <v>13</v>
       </c>
@@ -2010,7 +2038,7 @@
       <c r="AA18" s="9"/>
       <c r="AB18" s="9">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2035,8 +2063,12 @@
       <c r="K19" s="9">
         <v>6</v>
       </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="L19" s="9">
+        <v>17</v>
+      </c>
+      <c r="M19" s="9">
+        <v>22</v>
+      </c>
       <c r="N19" s="9">
         <v>4</v>
       </c>
@@ -2057,7 +2089,7 @@
       <c r="AA19" s="9"/>
       <c r="AB19" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2082,8 +2114,12 @@
       <c r="K20" s="9">
         <v>10</v>
       </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="L20" s="9">
+        <v>12</v>
+      </c>
+      <c r="M20" s="9">
+        <v>18</v>
+      </c>
       <c r="N20" s="9">
         <v>8</v>
       </c>
@@ -2104,7 +2140,7 @@
       <c r="AA20" s="9"/>
       <c r="AB20" s="9">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2129,8 +2165,12 @@
       <c r="K21" s="9">
         <v>29</v>
       </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="L21" s="9">
+        <v>22</v>
+      </c>
+      <c r="M21" s="9">
+        <v>34</v>
+      </c>
       <c r="N21" s="9">
         <v>15</v>
       </c>
@@ -2151,7 +2191,7 @@
       <c r="AA21" s="9"/>
       <c r="AB21" s="9">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2176,8 +2216,12 @@
       <c r="K22" s="9">
         <v>19</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
+      <c r="L22" s="9">
+        <v>22</v>
+      </c>
+      <c r="M22" s="9">
+        <v>7</v>
+      </c>
       <c r="N22" s="9">
         <v>11</v>
       </c>
@@ -2198,7 +2242,7 @@
       <c r="AA22" s="9"/>
       <c r="AB22" s="9">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2493,8 +2537,12 @@
       <c r="K29" s="9">
         <v>25</v>
       </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
+      <c r="L29" s="9">
+        <v>30</v>
+      </c>
+      <c r="M29" s="9">
+        <v>36</v>
+      </c>
       <c r="N29" s="9">
         <v>23</v>
       </c>
@@ -2515,7 +2563,7 @@
       <c r="AA29" s="9"/>
       <c r="AB29" s="9">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2569,8 +2617,12 @@
       <c r="K31" s="9">
         <v>24</v>
       </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
+      <c r="L31" s="9">
+        <v>12</v>
+      </c>
+      <c r="M31" s="9">
+        <v>16</v>
+      </c>
       <c r="N31" s="9">
         <v>17</v>
       </c>
@@ -2591,7 +2643,7 @@
       <c r="AA31" s="9"/>
       <c r="AB31" s="9">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2616,8 +2668,12 @@
       <c r="K32" s="9">
         <v>23</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
+      <c r="L32" s="9">
+        <v>10</v>
+      </c>
+      <c r="M32" s="9">
+        <v>24</v>
+      </c>
       <c r="N32" s="9">
         <v>25</v>
       </c>
@@ -2638,7 +2694,7 @@
       <c r="AA32" s="9"/>
       <c r="AB32" s="9">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2663,8 +2719,12 @@
       <c r="K33" s="9">
         <v>29</v>
       </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="L33" s="9">
+        <v>23</v>
+      </c>
+      <c r="M33" s="9">
+        <v>28</v>
+      </c>
       <c r="N33" s="9">
         <v>23</v>
       </c>
@@ -2685,7 +2745,7 @@
       <c r="AA33" s="9"/>
       <c r="AB33" s="9">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2710,8 +2770,12 @@
       <c r="K34" s="9">
         <v>25</v>
       </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
+      <c r="L34" s="9">
+        <v>17</v>
+      </c>
+      <c r="M34" s="9">
+        <v>13</v>
+      </c>
       <c r="N34" s="9">
         <v>25</v>
       </c>
@@ -2732,7 +2796,7 @@
       <c r="AA34" s="9"/>
       <c r="AB34" s="9">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2757,8 +2821,12 @@
       <c r="K35" s="9">
         <v>36</v>
       </c>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
+      <c r="L35" s="9">
+        <v>16</v>
+      </c>
+      <c r="M35" s="9">
+        <v>7</v>
+      </c>
       <c r="N35" s="9">
         <v>18</v>
       </c>
@@ -2779,7 +2847,7 @@
       <c r="AA35" s="9"/>
       <c r="AB35" s="9">
         <f t="shared" si="0"/>
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3122,8 +3190,12 @@
       <c r="K43" s="9">
         <v>33</v>
       </c>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
+      <c r="L43" s="9">
+        <v>26</v>
+      </c>
+      <c r="M43" s="9">
+        <v>27</v>
+      </c>
       <c r="N43" s="9">
         <v>32</v>
       </c>
@@ -3144,7 +3216,7 @@
       <c r="AA43" s="9"/>
       <c r="AB43" s="9">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3243,8 +3315,12 @@
       <c r="K46" s="9">
         <v>6</v>
       </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
+      <c r="L46" s="9">
+        <v>17</v>
+      </c>
+      <c r="M46" s="9">
+        <v>23</v>
+      </c>
       <c r="N46" s="9">
         <v>22</v>
       </c>
@@ -3265,7 +3341,7 @@
       <c r="AA46" s="9"/>
       <c r="AB46" s="9">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3290,8 +3366,12 @@
       <c r="K47" s="9">
         <v>7</v>
       </c>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
+      <c r="L47" s="9">
+        <v>10</v>
+      </c>
+      <c r="M47" s="9">
+        <v>16</v>
+      </c>
       <c r="N47" s="9">
         <v>23</v>
       </c>
@@ -3312,7 +3392,7 @@
       <c r="AA47" s="9"/>
       <c r="AB47" s="9">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3382,8 +3462,12 @@
       <c r="K49" s="9">
         <v>2</v>
       </c>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
+      <c r="L49" s="9">
+        <v>18</v>
+      </c>
+      <c r="M49" s="9">
+        <v>23</v>
+      </c>
       <c r="N49" s="9">
         <v>22</v>
       </c>
@@ -3404,7 +3488,7 @@
       <c r="AA49" s="9"/>
       <c r="AB49" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3429,8 +3513,12 @@
       <c r="K50" s="9">
         <v>0</v>
       </c>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
+      <c r="L50" s="9">
+        <v>16</v>
+      </c>
+      <c r="M50" s="9">
+        <v>20</v>
+      </c>
       <c r="N50" s="9">
         <v>28</v>
       </c>
@@ -3451,7 +3539,7 @@
       <c r="AA50" s="9"/>
       <c r="AB50" s="9">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3476,8 +3564,12 @@
       <c r="K51" s="9">
         <v>-6</v>
       </c>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
+      <c r="L51" s="9">
+        <v>12</v>
+      </c>
+      <c r="M51" s="9">
+        <v>22</v>
+      </c>
       <c r="N51" s="9">
         <v>21</v>
       </c>
@@ -3498,7 +3590,7 @@
       <c r="AA51" s="9"/>
       <c r="AB51" s="9">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3748,8 +3840,12 @@
       <c r="K57" s="9">
         <v>1</v>
       </c>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
+      <c r="L57" s="9">
+        <v>30</v>
+      </c>
+      <c r="M57" s="9">
+        <v>20</v>
+      </c>
       <c r="N57" s="9">
         <v>38</v>
       </c>
@@ -3770,7 +3866,7 @@
       <c r="AA57" s="9"/>
       <c r="AB57" s="9">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3824,8 +3920,12 @@
       <c r="K59" s="9">
         <v>9</v>
       </c>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
+      <c r="L59" s="9">
+        <v>9</v>
+      </c>
+      <c r="M59" s="9">
+        <v>10</v>
+      </c>
       <c r="N59" s="9">
         <v>19</v>
       </c>
@@ -3846,7 +3946,7 @@
       <c r="AA59" s="9"/>
       <c r="AB59" s="9">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3871,8 +3971,12 @@
       <c r="K60" s="9">
         <v>12</v>
       </c>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
+      <c r="L60" s="9">
+        <v>7</v>
+      </c>
+      <c r="M60" s="9">
+        <v>6</v>
+      </c>
       <c r="N60" s="9">
         <v>16</v>
       </c>
@@ -3893,7 +3997,7 @@
       <c r="AA60" s="9"/>
       <c r="AB60" s="9">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3918,8 +4022,12 @@
       <c r="K61" s="9">
         <v>23</v>
       </c>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
+      <c r="L61" s="9">
+        <v>20</v>
+      </c>
+      <c r="M61" s="9">
+        <v>0</v>
+      </c>
       <c r="N61" s="9">
         <v>12</v>
       </c>
@@ -3940,7 +4048,7 @@
       <c r="AA61" s="9"/>
       <c r="AB61" s="9">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3965,8 +4073,12 @@
       <c r="K62" s="9">
         <v>26</v>
       </c>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
+      <c r="L62" s="9">
+        <v>13</v>
+      </c>
+      <c r="M62" s="9">
+        <v>14</v>
+      </c>
       <c r="N62" s="9">
         <v>28</v>
       </c>
@@ -3987,7 +4099,7 @@
       <c r="AA62" s="9"/>
       <c r="AB62" s="9">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4012,8 +4124,12 @@
       <c r="K63" s="9">
         <v>11</v>
       </c>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
+      <c r="L63" s="9">
+        <v>10</v>
+      </c>
+      <c r="M63" s="9">
+        <v>2</v>
+      </c>
       <c r="N63" s="9">
         <v>13</v>
       </c>
@@ -4034,7 +4150,7 @@
       <c r="AA63" s="9"/>
       <c r="AB63" s="9">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4329,8 +4445,12 @@
       <c r="K70" s="9">
         <v>23</v>
       </c>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
+      <c r="L70" s="9">
+        <v>34</v>
+      </c>
+      <c r="M70" s="9">
+        <v>6</v>
+      </c>
       <c r="N70" s="9">
         <v>25</v>
       </c>
@@ -4351,7 +4471,7 @@
       <c r="AA70" s="9"/>
       <c r="AB70" s="9">
         <f t="shared" ref="AB70:AB133" si="1">SUM(J70:AA70)</f>
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4405,8 +4525,12 @@
       <c r="K72" s="9">
         <v>13</v>
       </c>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
+      <c r="L72" s="9">
+        <v>0</v>
+      </c>
+      <c r="M72" s="9">
+        <v>9</v>
+      </c>
       <c r="N72" s="9">
         <v>13</v>
       </c>
@@ -4427,7 +4551,7 @@
       <c r="AA72" s="9"/>
       <c r="AB72" s="9">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4452,8 +4576,12 @@
       <c r="K73" s="9">
         <v>16</v>
       </c>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
+      <c r="L73" s="9">
+        <v>3</v>
+      </c>
+      <c r="M73" s="9">
+        <v>11</v>
+      </c>
       <c r="N73" s="9">
         <v>13</v>
       </c>
@@ -4474,7 +4602,7 @@
       <c r="AA73" s="9"/>
       <c r="AB73" s="9">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4499,8 +4627,12 @@
       <c r="K74" s="9">
         <v>20</v>
       </c>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
+      <c r="L74" s="9">
+        <v>4</v>
+      </c>
+      <c r="M74" s="9">
+        <v>15</v>
+      </c>
       <c r="N74" s="9">
         <v>16</v>
       </c>
@@ -4521,7 +4653,7 @@
       <c r="AA74" s="9"/>
       <c r="AB74" s="9">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4546,8 +4678,12 @@
       <c r="K75" s="9">
         <v>26</v>
       </c>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
+      <c r="L75" s="9">
+        <v>7</v>
+      </c>
+      <c r="M75" s="9">
+        <v>18</v>
+      </c>
       <c r="N75" s="9">
         <v>9</v>
       </c>
@@ -4568,7 +4704,7 @@
       <c r="AA75" s="9"/>
       <c r="AB75" s="9">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4593,8 +4729,12 @@
       <c r="K76" s="9">
         <v>17</v>
       </c>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
+      <c r="L76" s="9">
+        <v>4</v>
+      </c>
+      <c r="M76" s="9">
+        <v>15</v>
+      </c>
       <c r="N76" s="9">
         <v>1</v>
       </c>
@@ -4615,7 +4755,7 @@
       <c r="AA76" s="9"/>
       <c r="AB76" s="9">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4910,8 +5050,12 @@
       <c r="K83" s="9">
         <v>28</v>
       </c>
-      <c r="L83" s="9"/>
-      <c r="M83" s="9"/>
+      <c r="L83" s="9">
+        <v>6</v>
+      </c>
+      <c r="M83" s="9">
+        <v>35</v>
+      </c>
       <c r="N83" s="9">
         <v>15</v>
       </c>
@@ -4932,7 +5076,7 @@
       <c r="AA83" s="9"/>
       <c r="AB83" s="9">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4986,8 +5130,12 @@
       <c r="K85" s="9">
         <v>2</v>
       </c>
-      <c r="L85" s="9"/>
-      <c r="M85" s="9"/>
+      <c r="L85" s="9">
+        <v>2</v>
+      </c>
+      <c r="M85" s="9">
+        <v>13</v>
+      </c>
       <c r="N85" s="9">
         <v>13</v>
       </c>
@@ -5008,7 +5156,7 @@
       <c r="AA85" s="9"/>
       <c r="AB85" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5033,8 +5181,12 @@
       <c r="K86" s="9">
         <v>5</v>
       </c>
-      <c r="L86" s="9"/>
-      <c r="M86" s="9"/>
+      <c r="L86" s="9">
+        <v>0</v>
+      </c>
+      <c r="M86" s="9">
+        <v>16</v>
+      </c>
       <c r="N86" s="9" t="s">
         <v>148</v>
       </c>
@@ -5055,7 +5207,7 @@
       <c r="AA86" s="9"/>
       <c r="AB86" s="9">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5080,8 +5232,12 @@
       <c r="K87" s="9">
         <v>-1</v>
       </c>
-      <c r="L87" s="9"/>
-      <c r="M87" s="9"/>
+      <c r="L87" s="9">
+        <v>1</v>
+      </c>
+      <c r="M87" s="9">
+        <v>21</v>
+      </c>
       <c r="N87" s="9">
         <v>-2</v>
       </c>
@@ -5102,7 +5258,7 @@
       <c r="AA87" s="9"/>
       <c r="AB87" s="9">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5127,8 +5283,12 @@
       <c r="K88" s="9">
         <v>7</v>
       </c>
-      <c r="L88" s="9"/>
-      <c r="M88" s="9"/>
+      <c r="L88" s="9">
+        <v>-1</v>
+      </c>
+      <c r="M88" s="9">
+        <v>12</v>
+      </c>
       <c r="N88" s="9">
         <v>2</v>
       </c>
@@ -5149,7 +5309,7 @@
       <c r="AA88" s="9"/>
       <c r="AB88" s="9">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5174,8 +5334,12 @@
       <c r="K89" s="9">
         <v>4</v>
       </c>
-      <c r="L89" s="9"/>
-      <c r="M89" s="9"/>
+      <c r="L89" s="9">
+        <v>-2</v>
+      </c>
+      <c r="M89" s="9">
+        <v>11</v>
+      </c>
       <c r="N89" s="9">
         <v>-6</v>
       </c>
@@ -5196,7 +5360,7 @@
       <c r="AA89" s="9"/>
       <c r="AB89" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5536,8 +5700,12 @@
       <c r="K97" s="9">
         <v>6</v>
       </c>
-      <c r="L97" s="9"/>
-      <c r="M97" s="9"/>
+      <c r="L97" s="9">
+        <v>1</v>
+      </c>
+      <c r="M97" s="9">
+        <v>5</v>
+      </c>
       <c r="N97" s="9">
         <v>3</v>
       </c>
@@ -5558,7 +5726,7 @@
       <c r="AA97" s="9"/>
       <c r="AB97" s="9">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5612,8 +5780,12 @@
       <c r="K99" s="9">
         <v>2</v>
       </c>
-      <c r="L99" s="9"/>
-      <c r="M99" s="9"/>
+      <c r="L99" s="9">
+        <v>0</v>
+      </c>
+      <c r="M99" s="9">
+        <v>6</v>
+      </c>
       <c r="N99" s="9">
         <v>0</v>
       </c>
@@ -5634,7 +5806,7 @@
       <c r="AA99" s="9"/>
       <c r="AB99" s="9">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5659,8 +5831,12 @@
       <c r="K100" s="9">
         <v>2</v>
       </c>
-      <c r="L100" s="9"/>
-      <c r="M100" s="9"/>
+      <c r="L100" s="9">
+        <v>3</v>
+      </c>
+      <c r="M100" s="9">
+        <v>8</v>
+      </c>
       <c r="N100" s="9">
         <v>-1</v>
       </c>
@@ -5681,7 +5857,7 @@
       <c r="AA100" s="9"/>
       <c r="AB100" s="9">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5706,8 +5882,12 @@
       <c r="K101" s="9">
         <v>-2</v>
       </c>
-      <c r="L101" s="9"/>
-      <c r="M101" s="9"/>
+      <c r="L101" s="9">
+        <v>3</v>
+      </c>
+      <c r="M101" s="9">
+        <v>5</v>
+      </c>
       <c r="N101" s="9">
         <v>-5</v>
       </c>
@@ -5728,7 +5908,7 @@
       <c r="AA101" s="9"/>
       <c r="AB101" s="9">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5753,8 +5933,12 @@
       <c r="K102" s="9">
         <v>13</v>
       </c>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
+      <c r="L102" s="9">
+        <v>2</v>
+      </c>
+      <c r="M102" s="9">
+        <v>11</v>
+      </c>
       <c r="N102" s="9">
         <v>2</v>
       </c>
@@ -5775,7 +5959,7 @@
       <c r="AA102" s="9"/>
       <c r="AB102" s="9">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5800,8 +5984,12 @@
       <c r="K103" s="9">
         <v>-1</v>
       </c>
-      <c r="L103" s="9"/>
-      <c r="M103" s="9"/>
+      <c r="L103" s="9">
+        <v>2</v>
+      </c>
+      <c r="M103" s="9">
+        <v>8</v>
+      </c>
       <c r="N103" s="9">
         <v>1</v>
       </c>
@@ -5822,7 +6010,7 @@
       <c r="AA103" s="9"/>
       <c r="AB103" s="9">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6117,8 +6305,12 @@
       <c r="K110" s="9">
         <v>7</v>
       </c>
-      <c r="L110" s="9"/>
-      <c r="M110" s="9"/>
+      <c r="L110" s="9">
+        <v>7</v>
+      </c>
+      <c r="M110" s="9">
+        <v>5</v>
+      </c>
       <c r="N110" s="9">
         <v>0</v>
       </c>
@@ -6139,7 +6331,7 @@
       <c r="AA110" s="9"/>
       <c r="AB110" s="9">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6193,8 +6385,12 @@
       <c r="K112" s="9">
         <v>12</v>
       </c>
-      <c r="L112" s="9"/>
-      <c r="M112" s="9"/>
+      <c r="L112" s="9">
+        <v>5</v>
+      </c>
+      <c r="M112" s="9">
+        <v>18</v>
+      </c>
       <c r="N112" s="9">
         <v>10</v>
       </c>
@@ -6215,7 +6411,7 @@
       <c r="AA112" s="9"/>
       <c r="AB112" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="113" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6240,8 +6436,12 @@
       <c r="K113" s="9">
         <v>13</v>
       </c>
-      <c r="L113" s="9"/>
-      <c r="M113" s="9"/>
+      <c r="L113" s="9">
+        <v>-1</v>
+      </c>
+      <c r="M113" s="9">
+        <v>10</v>
+      </c>
       <c r="N113" s="9">
         <v>14</v>
       </c>
@@ -6262,7 +6462,7 @@
       <c r="AA113" s="9"/>
       <c r="AB113" s="9">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6287,8 +6487,12 @@
       <c r="K114" s="9">
         <v>19</v>
       </c>
-      <c r="L114" s="9"/>
-      <c r="M114" s="9"/>
+      <c r="L114" s="9">
+        <v>9</v>
+      </c>
+      <c r="M114" s="9">
+        <v>14</v>
+      </c>
       <c r="N114" s="9">
         <v>15</v>
       </c>
@@ -6309,7 +6513,7 @@
       <c r="AA114" s="9"/>
       <c r="AB114" s="9">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6334,8 +6538,12 @@
       <c r="K115" s="9">
         <v>9</v>
       </c>
-      <c r="L115" s="9"/>
-      <c r="M115" s="9"/>
+      <c r="L115" s="9">
+        <v>5</v>
+      </c>
+      <c r="M115" s="9">
+        <v>8</v>
+      </c>
       <c r="N115" s="9">
         <v>19</v>
       </c>
@@ -6356,7 +6564,7 @@
       <c r="AA115" s="9"/>
       <c r="AB115" s="9">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6381,8 +6589,12 @@
       <c r="K116" s="9">
         <v>19</v>
       </c>
-      <c r="L116" s="9"/>
-      <c r="M116" s="9"/>
+      <c r="L116" s="9">
+        <v>4</v>
+      </c>
+      <c r="M116" s="9">
+        <v>21</v>
+      </c>
       <c r="N116" s="9">
         <v>11</v>
       </c>
@@ -6403,7 +6615,7 @@
       <c r="AA116" s="9"/>
       <c r="AB116" s="9">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="117" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6698,8 +6910,12 @@
       <c r="K123" s="9">
         <v>35</v>
       </c>
-      <c r="L123" s="9"/>
-      <c r="M123" s="9"/>
+      <c r="L123" s="9">
+        <v>6</v>
+      </c>
+      <c r="M123" s="9">
+        <v>39</v>
+      </c>
       <c r="N123" s="9">
         <v>35</v>
       </c>
@@ -6720,7 +6936,7 @@
       <c r="AA123" s="9"/>
       <c r="AB123" s="9">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>155</v>
       </c>
     </row>
     <row r="124" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6774,8 +6990,12 @@
       <c r="K125" s="9">
         <v>3</v>
       </c>
-      <c r="L125" s="9"/>
-      <c r="M125" s="9"/>
+      <c r="L125" s="9">
+        <v>2</v>
+      </c>
+      <c r="M125" s="9">
+        <v>3</v>
+      </c>
       <c r="N125" s="9">
         <v>1</v>
       </c>
@@ -6796,7 +7016,7 @@
       <c r="AA125" s="9"/>
       <c r="AB125" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6866,8 +7086,12 @@
       <c r="K127" s="9">
         <v>14</v>
       </c>
-      <c r="L127" s="9"/>
-      <c r="M127" s="9"/>
+      <c r="L127" s="9">
+        <v>2</v>
+      </c>
+      <c r="M127" s="9">
+        <v>1</v>
+      </c>
       <c r="N127" s="9">
         <v>4</v>
       </c>
@@ -6888,7 +7112,7 @@
       <c r="AA127" s="9"/>
       <c r="AB127" s="9">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6958,8 +7182,12 @@
       <c r="K129" s="9">
         <v>9</v>
       </c>
-      <c r="L129" s="9"/>
-      <c r="M129" s="9"/>
+      <c r="L129" s="9">
+        <v>-1</v>
+      </c>
+      <c r="M129" s="9">
+        <v>2</v>
+      </c>
       <c r="N129" s="9">
         <v>4</v>
       </c>
@@ -6980,7 +7208,7 @@
       <c r="AA129" s="9"/>
       <c r="AB129" s="9">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7005,8 +7233,12 @@
       <c r="K130" s="9">
         <v>3</v>
       </c>
-      <c r="L130" s="9"/>
-      <c r="M130" s="9"/>
+      <c r="L130" s="9">
+        <v>-2</v>
+      </c>
+      <c r="M130" s="9">
+        <v>0</v>
+      </c>
       <c r="N130" s="9">
         <v>0</v>
       </c>
@@ -7027,7 +7259,7 @@
       <c r="AA130" s="9"/>
       <c r="AB130" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7142,8 +7374,12 @@
       <c r="K133" s="9">
         <v>10</v>
       </c>
-      <c r="L133" s="9"/>
-      <c r="M133" s="9"/>
+      <c r="L133" s="9">
+        <v>-6</v>
+      </c>
+      <c r="M133" s="9">
+        <v>-1</v>
+      </c>
       <c r="N133" s="9">
         <v>4</v>
       </c>
@@ -7164,7 +7400,7 @@
       <c r="AA133" s="9"/>
       <c r="AB133" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="134" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7369,8 +7605,12 @@
       <c r="K138" s="9">
         <v>8</v>
       </c>
-      <c r="L138" s="9"/>
-      <c r="M138" s="9"/>
+      <c r="L138" s="9">
+        <v>1</v>
+      </c>
+      <c r="M138" s="9">
+        <v>2</v>
+      </c>
       <c r="N138" s="9">
         <v>3</v>
       </c>
@@ -7391,7 +7631,7 @@
       <c r="AA138" s="9"/>
       <c r="AB138" s="9">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="139" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
semana 4 en lec.xlsx
</commit_message>
<xml_diff>
--- a/LEC.xlsx
+++ b/LEC.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="158">
   <si>
     <t>EQUIPO</t>
   </si>
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:AC705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M64" sqref="M64"/>
+    <sheetView tabSelected="1" topLeftCell="F97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R122" sqref="R122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1419,8 +1419,12 @@
       <c r="O5" s="9">
         <v>14</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="P5" s="9">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>9</v>
+      </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
@@ -1433,7 +1437,7 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9">
         <f>SUM(J5:AA5)</f>
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1470,8 +1474,12 @@
       <c r="O6" s="9">
         <v>7</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
+      <c r="P6" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>-2</v>
+      </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -1484,7 +1492,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9">
         <f t="shared" ref="AB6:AB69" si="0">SUM(J6:AA6)</f>
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1521,8 +1529,12 @@
       <c r="O7" s="9">
         <v>21</v>
       </c>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
+      <c r="P7" s="9">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>6</v>
+      </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
@@ -1535,7 +1547,7 @@
       <c r="AA7" s="9"/>
       <c r="AB7" s="9">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1572,8 +1584,12 @@
       <c r="O8" s="9">
         <v>15</v>
       </c>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
+      <c r="P8" s="9">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>6</v>
+      </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
@@ -1586,7 +1602,7 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1623,8 +1639,12 @@
       <c r="O9" s="9">
         <v>18</v>
       </c>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="P9" s="9">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>3</v>
+      </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
@@ -1637,7 +1657,7 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1944,8 +1964,12 @@
       <c r="O16" s="9">
         <v>33</v>
       </c>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="P16" s="9">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>7</v>
+      </c>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
@@ -1958,7 +1982,7 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2024,8 +2048,12 @@
       <c r="O18" s="9">
         <v>6</v>
       </c>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="P18" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>6</v>
+      </c>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
@@ -2038,7 +2066,7 @@
       <c r="AA18" s="9"/>
       <c r="AB18" s="9">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2075,8 +2103,12 @@
       <c r="O19" s="9">
         <v>9</v>
       </c>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="P19" s="9">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>7</v>
+      </c>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
@@ -2089,7 +2121,7 @@
       <c r="AA19" s="9"/>
       <c r="AB19" s="9">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2126,8 +2158,12 @@
       <c r="O20" s="9">
         <v>3</v>
       </c>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="P20" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>4</v>
+      </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
@@ -2140,7 +2176,7 @@
       <c r="AA20" s="9"/>
       <c r="AB20" s="9">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2177,8 +2213,12 @@
       <c r="O21" s="9">
         <v>3</v>
       </c>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="P21" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>8</v>
+      </c>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
@@ -2191,7 +2231,7 @@
       <c r="AA21" s="9"/>
       <c r="AB21" s="9">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2228,8 +2268,12 @@
       <c r="O22" s="9">
         <v>-3</v>
       </c>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="P22" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>-4</v>
+      </c>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
@@ -2242,7 +2286,7 @@
       <c r="AA22" s="9"/>
       <c r="AB22" s="9">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2549,8 +2593,12 @@
       <c r="O29" s="9">
         <v>5</v>
       </c>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="P29" s="9">
+        <v>38</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>4</v>
+      </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
@@ -2563,7 +2611,7 @@
       <c r="AA29" s="9"/>
       <c r="AB29" s="9">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2629,8 +2677,12 @@
       <c r="O31" s="9">
         <v>20</v>
       </c>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="P31" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>5</v>
+      </c>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
@@ -2643,7 +2695,7 @@
       <c r="AA31" s="9"/>
       <c r="AB31" s="9">
         <f t="shared" si="0"/>
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2680,8 +2732,12 @@
       <c r="O32" s="9">
         <v>21</v>
       </c>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
+      <c r="P32" s="9">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>4</v>
+      </c>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
@@ -2694,7 +2750,7 @@
       <c r="AA32" s="9"/>
       <c r="AB32" s="9">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2731,8 +2787,12 @@
       <c r="O33" s="9">
         <v>31</v>
       </c>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
+      <c r="P33" s="9">
+        <v>-5</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>9</v>
+      </c>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
@@ -2745,7 +2805,7 @@
       <c r="AA33" s="9"/>
       <c r="AB33" s="9">
         <f t="shared" si="0"/>
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2782,8 +2842,12 @@
       <c r="O34" s="9">
         <v>18</v>
       </c>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
+      <c r="P34" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="9">
+        <v>4</v>
+      </c>
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
@@ -2796,7 +2860,7 @@
       <c r="AA34" s="9"/>
       <c r="AB34" s="9">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2833,8 +2897,12 @@
       <c r="O35" s="9">
         <v>33</v>
       </c>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
+      <c r="P35" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>0</v>
+      </c>
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
@@ -2847,7 +2915,7 @@
       <c r="AA35" s="9"/>
       <c r="AB35" s="9">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3202,8 +3270,12 @@
       <c r="O43" s="9">
         <v>27</v>
       </c>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
+      <c r="P43" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="9">
+        <v>19</v>
+      </c>
       <c r="R43" s="9"/>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
@@ -3216,7 +3288,7 @@
       <c r="AA43" s="9"/>
       <c r="AB43" s="9">
         <f t="shared" si="0"/>
-        <v>179</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3327,8 +3399,12 @@
       <c r="O46" s="9">
         <v>11</v>
       </c>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
+      <c r="P46" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q46" s="9">
+        <v>20</v>
+      </c>
       <c r="R46" s="9"/>
       <c r="S46" s="9"/>
       <c r="T46" s="9"/>
@@ -3341,7 +3417,7 @@
       <c r="AA46" s="9"/>
       <c r="AB46" s="9">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3378,8 +3454,12 @@
       <c r="O47" s="9">
         <v>16</v>
       </c>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
+      <c r="P47" s="9">
+        <v>23</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>8</v>
+      </c>
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
       <c r="T47" s="9"/>
@@ -3392,7 +3472,7 @@
       <c r="AA47" s="9"/>
       <c r="AB47" s="9">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3474,8 +3554,12 @@
       <c r="O49" s="9">
         <v>14</v>
       </c>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
+      <c r="P49" s="9">
+        <v>23</v>
+      </c>
+      <c r="Q49" s="9">
+        <v>16</v>
+      </c>
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
@@ -3488,7 +3572,7 @@
       <c r="AA49" s="9"/>
       <c r="AB49" s="9">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3525,8 +3609,12 @@
       <c r="O50" s="9">
         <v>22</v>
       </c>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
+      <c r="P50" s="9">
+        <v>23</v>
+      </c>
+      <c r="Q50" s="9">
+        <v>11</v>
+      </c>
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
       <c r="T50" s="9"/>
@@ -3539,7 +3627,7 @@
       <c r="AA50" s="9"/>
       <c r="AB50" s="9">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3576,8 +3664,12 @@
       <c r="O51" s="9">
         <v>17</v>
       </c>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="9"/>
+      <c r="P51" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q51" s="9">
+        <v>15</v>
+      </c>
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
       <c r="T51" s="9"/>
@@ -3590,7 +3682,7 @@
       <c r="AA51" s="9"/>
       <c r="AB51" s="9">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3852,8 +3944,12 @@
       <c r="O57" s="9">
         <v>26</v>
       </c>
-      <c r="P57" s="9"/>
-      <c r="Q57" s="9"/>
+      <c r="P57" s="9">
+        <v>35</v>
+      </c>
+      <c r="Q57" s="9">
+        <v>42</v>
+      </c>
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
       <c r="T57" s="9"/>
@@ -3866,7 +3962,7 @@
       <c r="AA57" s="9"/>
       <c r="AB57" s="9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3932,8 +4028,12 @@
       <c r="O59" s="9">
         <v>5</v>
       </c>
-      <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
+      <c r="P59" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q59" s="9">
+        <v>30</v>
+      </c>
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
@@ -3946,7 +4046,7 @@
       <c r="AA59" s="9"/>
       <c r="AB59" s="9">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3983,8 +4083,12 @@
       <c r="O60" s="9">
         <v>8</v>
       </c>
-      <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
+      <c r="P60" s="9">
+        <v>25</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>14</v>
+      </c>
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
       <c r="T60" s="9"/>
@@ -3997,7 +4101,7 @@
       <c r="AA60" s="9"/>
       <c r="AB60" s="9">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4034,8 +4138,12 @@
       <c r="O61" s="9">
         <v>5</v>
       </c>
-      <c r="P61" s="9"/>
-      <c r="Q61" s="9"/>
+      <c r="P61" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q61" s="9">
+        <v>22</v>
+      </c>
       <c r="R61" s="9"/>
       <c r="S61" s="9"/>
       <c r="T61" s="9"/>
@@ -4048,7 +4156,7 @@
       <c r="AA61" s="9"/>
       <c r="AB61" s="9">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4085,8 +4193,12 @@
       <c r="O62" s="9">
         <v>7</v>
       </c>
-      <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
+      <c r="P62" s="9">
+        <v>21</v>
+      </c>
+      <c r="Q62" s="9">
+        <v>18</v>
+      </c>
       <c r="R62" s="9"/>
       <c r="S62" s="9"/>
       <c r="T62" s="9"/>
@@ -4099,7 +4211,7 @@
       <c r="AA62" s="9"/>
       <c r="AB62" s="9">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4136,8 +4248,12 @@
       <c r="O63" s="9">
         <v>6</v>
       </c>
-      <c r="P63" s="9"/>
-      <c r="Q63" s="9"/>
+      <c r="P63" s="9">
+        <v>25</v>
+      </c>
+      <c r="Q63" s="9">
+        <v>10</v>
+      </c>
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
       <c r="T63" s="9"/>
@@ -4150,7 +4266,7 @@
       <c r="AA63" s="9"/>
       <c r="AB63" s="9">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4457,8 +4573,12 @@
       <c r="O70" s="9">
         <v>14</v>
       </c>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="9"/>
+      <c r="P70" s="9">
+        <v>31</v>
+      </c>
+      <c r="Q70" s="9">
+        <v>33</v>
+      </c>
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
       <c r="T70" s="9"/>
@@ -4471,7 +4591,7 @@
       <c r="AA70" s="9"/>
       <c r="AB70" s="9">
         <f t="shared" ref="AB70:AB133" si="1">SUM(J70:AA70)</f>
-        <v>135</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4537,8 +4657,12 @@
       <c r="O72" s="9">
         <v>1</v>
       </c>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
+      <c r="P72" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q72" s="9">
+        <v>10</v>
+      </c>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
@@ -4551,7 +4675,7 @@
       <c r="AA72" s="9"/>
       <c r="AB72" s="9">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4588,8 +4712,12 @@
       <c r="O73" s="9">
         <v>3</v>
       </c>
-      <c r="P73" s="9"/>
-      <c r="Q73" s="9"/>
+      <c r="P73" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q73" s="9">
+        <v>15</v>
+      </c>
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
@@ -4602,7 +4730,7 @@
       <c r="AA73" s="9"/>
       <c r="AB73" s="9">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4639,8 +4767,12 @@
       <c r="O74" s="9">
         <v>1</v>
       </c>
-      <c r="P74" s="9"/>
-      <c r="Q74" s="9"/>
+      <c r="P74" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q74" s="9">
+        <v>9</v>
+      </c>
       <c r="R74" s="9"/>
       <c r="S74" s="9"/>
       <c r="T74" s="9"/>
@@ -4653,7 +4785,7 @@
       <c r="AA74" s="9"/>
       <c r="AB74" s="9">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4690,8 +4822,12 @@
       <c r="O75" s="9">
         <v>12</v>
       </c>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
+      <c r="P75" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q75" s="9">
+        <v>12</v>
+      </c>
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
       <c r="T75" s="9"/>
@@ -4704,7 +4840,7 @@
       <c r="AA75" s="9"/>
       <c r="AB75" s="9">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4741,8 +4877,12 @@
       <c r="O76" s="9">
         <v>9</v>
       </c>
-      <c r="P76" s="9"/>
-      <c r="Q76" s="9"/>
+      <c r="P76" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>16</v>
+      </c>
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
       <c r="T76" s="9"/>
@@ -4755,7 +4895,7 @@
       <c r="AA76" s="9"/>
       <c r="AB76" s="9">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5062,8 +5202,12 @@
       <c r="O83" s="9">
         <v>19</v>
       </c>
-      <c r="P83" s="9"/>
-      <c r="Q83" s="9"/>
+      <c r="P83" s="9">
+        <v>29</v>
+      </c>
+      <c r="Q83" s="9">
+        <v>34</v>
+      </c>
       <c r="R83" s="9"/>
       <c r="S83" s="9"/>
       <c r="T83" s="9"/>
@@ -5076,7 +5220,7 @@
       <c r="AA83" s="9"/>
       <c r="AB83" s="9">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5142,8 +5286,12 @@
       <c r="O85" s="9">
         <v>1</v>
       </c>
-      <c r="P85" s="9"/>
-      <c r="Q85" s="9"/>
+      <c r="P85" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>28</v>
+      </c>
       <c r="R85" s="9"/>
       <c r="S85" s="9"/>
       <c r="T85" s="9"/>
@@ -5156,7 +5304,7 @@
       <c r="AA85" s="9"/>
       <c r="AB85" s="9">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5193,7 +5341,9 @@
       <c r="O86" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="P86" s="9"/>
+      <c r="P86" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="Q86" s="9"/>
       <c r="R86" s="9"/>
       <c r="S86" s="9"/>
@@ -5244,8 +5394,12 @@
       <c r="O87" s="9">
         <v>2</v>
       </c>
-      <c r="P87" s="9"/>
-      <c r="Q87" s="9"/>
+      <c r="P87" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q87" s="9">
+        <v>21</v>
+      </c>
       <c r="R87" s="9"/>
       <c r="S87" s="9"/>
       <c r="T87" s="9"/>
@@ -5258,7 +5412,7 @@
       <c r="AA87" s="9"/>
       <c r="AB87" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5295,8 +5449,12 @@
       <c r="O88" s="9">
         <v>5</v>
       </c>
-      <c r="P88" s="9"/>
-      <c r="Q88" s="9"/>
+      <c r="P88" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q88" s="9">
+        <v>30</v>
+      </c>
       <c r="R88" s="9"/>
       <c r="S88" s="9"/>
       <c r="T88" s="9"/>
@@ -5309,7 +5467,7 @@
       <c r="AA88" s="9"/>
       <c r="AB88" s="9">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5346,8 +5504,12 @@
       <c r="O89" s="9">
         <v>5</v>
       </c>
-      <c r="P89" s="9"/>
-      <c r="Q89" s="9"/>
+      <c r="P89" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q89" s="9">
+        <v>22</v>
+      </c>
       <c r="R89" s="9"/>
       <c r="S89" s="9"/>
       <c r="T89" s="9"/>
@@ -5360,7 +5522,7 @@
       <c r="AA89" s="9"/>
       <c r="AB89" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5436,8 +5598,12 @@
       <c r="O91" s="9">
         <v>6</v>
       </c>
-      <c r="P91" s="9"/>
-      <c r="Q91" s="9"/>
+      <c r="P91" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="9">
+        <v>21</v>
+      </c>
       <c r="R91" s="9"/>
       <c r="S91" s="9"/>
       <c r="T91" s="9"/>
@@ -5450,7 +5616,7 @@
       <c r="AA91" s="9"/>
       <c r="AB91" s="9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5712,7 +5878,9 @@
       <c r="O97" s="9">
         <v>8</v>
       </c>
-      <c r="P97" s="9"/>
+      <c r="P97" s="9">
+        <v>4</v>
+      </c>
       <c r="Q97" s="9"/>
       <c r="R97" s="9"/>
       <c r="S97" s="9"/>
@@ -5726,7 +5894,7 @@
       <c r="AA97" s="9"/>
       <c r="AB97" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5792,8 +5960,12 @@
       <c r="O99" s="9">
         <v>16</v>
       </c>
-      <c r="P99" s="9"/>
-      <c r="Q99" s="9"/>
+      <c r="P99" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q99" s="9">
+        <v>-1</v>
+      </c>
       <c r="R99" s="9"/>
       <c r="S99" s="9"/>
       <c r="T99" s="9"/>
@@ -5806,7 +5978,7 @@
       <c r="AA99" s="9"/>
       <c r="AB99" s="9">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5843,8 +6015,12 @@
       <c r="O100" s="9">
         <v>22</v>
       </c>
-      <c r="P100" s="9"/>
-      <c r="Q100" s="9"/>
+      <c r="P100" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q100" s="9">
+        <v>0</v>
+      </c>
       <c r="R100" s="9"/>
       <c r="S100" s="9"/>
       <c r="T100" s="9"/>
@@ -5857,7 +6033,7 @@
       <c r="AA100" s="9"/>
       <c r="AB100" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5894,8 +6070,12 @@
       <c r="O101" s="9">
         <v>17</v>
       </c>
-      <c r="P101" s="9"/>
-      <c r="Q101" s="9"/>
+      <c r="P101" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q101" s="9">
+        <v>3</v>
+      </c>
       <c r="R101" s="9"/>
       <c r="S101" s="9"/>
       <c r="T101" s="9"/>
@@ -5908,7 +6088,7 @@
       <c r="AA101" s="9"/>
       <c r="AB101" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5945,8 +6125,12 @@
       <c r="O102" s="9">
         <v>23</v>
       </c>
-      <c r="P102" s="9"/>
-      <c r="Q102" s="9"/>
+      <c r="P102" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q102" s="9">
+        <v>8</v>
+      </c>
       <c r="R102" s="9"/>
       <c r="S102" s="9"/>
       <c r="T102" s="9"/>
@@ -5959,7 +6143,7 @@
       <c r="AA102" s="9"/>
       <c r="AB102" s="9">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5996,8 +6180,12 @@
       <c r="O103" s="9">
         <v>17</v>
       </c>
-      <c r="P103" s="9"/>
-      <c r="Q103" s="9"/>
+      <c r="P103" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="9">
+        <v>3</v>
+      </c>
       <c r="R103" s="9"/>
       <c r="S103" s="9"/>
       <c r="T103" s="9"/>
@@ -6010,7 +6198,7 @@
       <c r="AA103" s="9"/>
       <c r="AB103" s="9">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6317,8 +6505,12 @@
       <c r="O110" s="9">
         <v>39</v>
       </c>
-      <c r="P110" s="9"/>
-      <c r="Q110" s="9"/>
+      <c r="P110" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q110" s="9">
+        <v>1</v>
+      </c>
       <c r="R110" s="9"/>
       <c r="S110" s="9"/>
       <c r="T110" s="9"/>
@@ -6331,7 +6523,7 @@
       <c r="AA110" s="9"/>
       <c r="AB110" s="9">
         <f t="shared" si="1"/>
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6397,8 +6589,12 @@
       <c r="O112" s="9">
         <v>20</v>
       </c>
-      <c r="P112" s="9"/>
-      <c r="Q112" s="9"/>
+      <c r="P112" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="9">
+        <v>27</v>
+      </c>
       <c r="R112" s="9"/>
       <c r="S112" s="9"/>
       <c r="T112" s="9"/>
@@ -6411,7 +6607,7 @@
       <c r="AA112" s="9"/>
       <c r="AB112" s="9">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6448,8 +6644,12 @@
       <c r="O113" s="9">
         <v>22</v>
       </c>
-      <c r="P113" s="9"/>
-      <c r="Q113" s="9"/>
+      <c r="P113" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="9">
+        <v>26</v>
+      </c>
       <c r="R113" s="9"/>
       <c r="S113" s="9"/>
       <c r="T113" s="9"/>
@@ -6462,7 +6662,7 @@
       <c r="AA113" s="9"/>
       <c r="AB113" s="9">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6499,8 +6699,12 @@
       <c r="O114" s="9">
         <v>21</v>
       </c>
-      <c r="P114" s="9"/>
-      <c r="Q114" s="9"/>
+      <c r="P114" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q114" s="9">
+        <v>22</v>
+      </c>
       <c r="R114" s="9"/>
       <c r="S114" s="9"/>
       <c r="T114" s="9"/>
@@ -6513,7 +6717,7 @@
       <c r="AA114" s="9"/>
       <c r="AB114" s="9">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6550,8 +6754,12 @@
       <c r="O115" s="9">
         <v>17</v>
       </c>
-      <c r="P115" s="9"/>
-      <c r="Q115" s="9"/>
+      <c r="P115" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q115" s="9">
+        <v>17</v>
+      </c>
       <c r="R115" s="9"/>
       <c r="S115" s="9"/>
       <c r="T115" s="9"/>
@@ -6564,7 +6772,7 @@
       <c r="AA115" s="9"/>
       <c r="AB115" s="9">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="116" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6601,8 +6809,12 @@
       <c r="O116" s="9">
         <v>22</v>
       </c>
-      <c r="P116" s="9"/>
-      <c r="Q116" s="9"/>
+      <c r="P116" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q116" s="9">
+        <v>4</v>
+      </c>
       <c r="R116" s="9"/>
       <c r="S116" s="9"/>
       <c r="T116" s="9"/>
@@ -6615,7 +6827,7 @@
       <c r="AA116" s="9"/>
       <c r="AB116" s="9">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6922,8 +7134,12 @@
       <c r="O123" s="9">
         <v>31</v>
       </c>
-      <c r="P123" s="9"/>
-      <c r="Q123" s="9"/>
+      <c r="P123" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q123" s="9">
+        <v>46</v>
+      </c>
       <c r="R123" s="9"/>
       <c r="S123" s="9"/>
       <c r="T123" s="9"/>
@@ -6936,7 +7152,7 @@
       <c r="AA123" s="9"/>
       <c r="AB123" s="9">
         <f t="shared" si="1"/>
-        <v>155</v>
+        <v>208</v>
       </c>
     </row>
     <row r="124" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7002,8 +7218,12 @@
       <c r="O125" s="9">
         <v>11</v>
       </c>
-      <c r="P125" s="9"/>
-      <c r="Q125" s="9"/>
+      <c r="P125" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q125" s="9">
+        <v>4</v>
+      </c>
       <c r="R125" s="9"/>
       <c r="S125" s="9"/>
       <c r="T125" s="9"/>
@@ -7016,7 +7236,7 @@
       <c r="AA125" s="9"/>
       <c r="AB125" s="9">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="126" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7047,7 +7267,9 @@
       <c r="O126" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="P126" s="9"/>
+      <c r="P126" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="Q126" s="9"/>
       <c r="R126" s="9"/>
       <c r="S126" s="9"/>
@@ -7098,8 +7320,12 @@
       <c r="O127" s="9">
         <v>7</v>
       </c>
-      <c r="P127" s="9"/>
-      <c r="Q127" s="9"/>
+      <c r="P127" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q127" s="9">
+        <v>1</v>
+      </c>
       <c r="R127" s="9"/>
       <c r="S127" s="9"/>
       <c r="T127" s="9"/>
@@ -7112,7 +7338,7 @@
       <c r="AA127" s="9"/>
       <c r="AB127" s="9">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="128" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7194,8 +7420,12 @@
       <c r="O129" s="9">
         <v>9</v>
       </c>
-      <c r="P129" s="9"/>
-      <c r="Q129" s="9"/>
+      <c r="P129" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q129" s="9">
+        <v>3</v>
+      </c>
       <c r="R129" s="9"/>
       <c r="S129" s="9"/>
       <c r="T129" s="9"/>
@@ -7208,7 +7438,7 @@
       <c r="AA129" s="9"/>
       <c r="AB129" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7245,8 +7475,12 @@
       <c r="O130" s="9">
         <v>7</v>
       </c>
-      <c r="P130" s="9"/>
-      <c r="Q130" s="9"/>
+      <c r="P130" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="9">
+        <v>6</v>
+      </c>
       <c r="R130" s="9"/>
       <c r="S130" s="9"/>
       <c r="T130" s="9"/>
@@ -7259,7 +7493,7 @@
       <c r="AA130" s="9"/>
       <c r="AB130" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7386,8 +7620,12 @@
       <c r="O133" s="9">
         <v>3</v>
       </c>
-      <c r="P133" s="9"/>
-      <c r="Q133" s="9"/>
+      <c r="P133" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q133" s="9">
+        <v>6</v>
+      </c>
       <c r="R133" s="9"/>
       <c r="S133" s="9"/>
       <c r="T133" s="9"/>
@@ -7400,7 +7638,7 @@
       <c r="AA133" s="9"/>
       <c r="AB133" s="9">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="134" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7617,8 +7855,12 @@
       <c r="O138" s="9">
         <v>12</v>
       </c>
-      <c r="P138" s="9"/>
-      <c r="Q138" s="9"/>
+      <c r="P138" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q138" s="9">
+        <v>2</v>
+      </c>
       <c r="R138" s="9"/>
       <c r="S138" s="9"/>
       <c r="T138" s="9"/>
@@ -7631,7 +7873,7 @@
       <c r="AA138" s="9"/>
       <c r="AB138" s="9">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="139" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
añadida la semana 6
</commit_message>
<xml_diff>
--- a/LEC.xlsx
+++ b/LEC.xlsx
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:AC705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R122" sqref="R122"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1427,8 +1427,12 @@
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="T5" s="9">
+        <v>-8</v>
+      </c>
+      <c r="U5" s="9">
+        <v>16</v>
+      </c>
       <c r="V5" s="9"/>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
@@ -1437,7 +1441,7 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9">
         <f>SUM(J5:AA5)</f>
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1482,8 +1486,12 @@
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
+      <c r="T6" s="9">
+        <v>-1</v>
+      </c>
+      <c r="U6" s="9">
+        <v>23</v>
+      </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
@@ -1492,7 +1500,7 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9">
         <f t="shared" ref="AB6:AB69" si="0">SUM(J6:AA6)</f>
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1537,8 +1545,12 @@
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
+      <c r="T7" s="9">
+        <v>4</v>
+      </c>
+      <c r="U7" s="9">
+        <v>20</v>
+      </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
@@ -1547,7 +1559,7 @@
       <c r="AA7" s="9"/>
       <c r="AB7" s="9">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1592,8 +1604,12 @@
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
+      <c r="T8" s="9">
+        <v>3</v>
+      </c>
+      <c r="U8" s="9">
+        <v>18</v>
+      </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
       <c r="X8" s="9"/>
@@ -1602,7 +1618,7 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1647,8 +1663,12 @@
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
+      <c r="T9" s="9">
+        <v>-1</v>
+      </c>
+      <c r="U9" s="9">
+        <v>21</v>
+      </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
@@ -1657,7 +1677,7 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1972,8 +1992,12 @@
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
+      <c r="T16" s="9">
+        <v>2</v>
+      </c>
+      <c r="U16" s="9">
+        <v>31</v>
+      </c>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
@@ -1982,7 +2006,7 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2056,8 +2080,12 @@
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
+      <c r="T18" s="9">
+        <v>11</v>
+      </c>
+      <c r="U18" s="9">
+        <v>10</v>
+      </c>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="9"/>
@@ -2066,7 +2094,7 @@
       <c r="AA18" s="9"/>
       <c r="AB18" s="9">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2111,8 +2139,12 @@
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
+      <c r="T19" s="9">
+        <v>13</v>
+      </c>
+      <c r="U19" s="9">
+        <v>8</v>
+      </c>
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
@@ -2121,7 +2153,7 @@
       <c r="AA19" s="9"/>
       <c r="AB19" s="9">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2166,8 +2198,12 @@
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
+      <c r="T20" s="9">
+        <v>31</v>
+      </c>
+      <c r="U20" s="9">
+        <v>14</v>
+      </c>
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
@@ -2176,7 +2212,7 @@
       <c r="AA20" s="9"/>
       <c r="AB20" s="9">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2221,8 +2257,12 @@
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
+      <c r="T21" s="9">
+        <v>18</v>
+      </c>
+      <c r="U21" s="9">
+        <v>27</v>
+      </c>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
@@ -2231,7 +2271,7 @@
       <c r="AA21" s="9"/>
       <c r="AB21" s="9">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2276,8 +2316,12 @@
       </c>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
+      <c r="T22" s="9">
+        <v>16</v>
+      </c>
+      <c r="U22" s="9">
+        <v>21</v>
+      </c>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9"/>
@@ -2286,7 +2330,7 @@
       <c r="AA22" s="9"/>
       <c r="AB22" s="9">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2601,8 +2645,12 @@
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
+      <c r="T29" s="9">
+        <v>33</v>
+      </c>
+      <c r="U29" s="9">
+        <v>34</v>
+      </c>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
@@ -2611,7 +2659,7 @@
       <c r="AA29" s="9"/>
       <c r="AB29" s="9">
         <f t="shared" si="0"/>
-        <v>172</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2685,8 +2733,12 @@
       </c>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
+      <c r="T31" s="9">
+        <v>20</v>
+      </c>
+      <c r="U31" s="9">
+        <v>18</v>
+      </c>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
@@ -2695,7 +2747,7 @@
       <c r="AA31" s="9"/>
       <c r="AB31" s="9">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2740,8 +2792,12 @@
       </c>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
+      <c r="T32" s="9">
+        <v>14</v>
+      </c>
+      <c r="U32" s="9">
+        <v>16</v>
+      </c>
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
@@ -2750,7 +2806,7 @@
       <c r="AA32" s="9"/>
       <c r="AB32" s="9">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2795,8 +2851,12 @@
       </c>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
+      <c r="T33" s="9">
+        <v>18</v>
+      </c>
+      <c r="U33" s="9">
+        <v>22</v>
+      </c>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
@@ -2805,7 +2865,7 @@
       <c r="AA33" s="9"/>
       <c r="AB33" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2850,8 +2910,12 @@
       </c>
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
+      <c r="T34" s="9">
+        <v>29</v>
+      </c>
+      <c r="U34" s="9">
+        <v>19</v>
+      </c>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
       <c r="X34" s="9"/>
@@ -2860,7 +2924,7 @@
       <c r="AA34" s="9"/>
       <c r="AB34" s="9">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2905,8 +2969,12 @@
       </c>
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
+      <c r="T35" s="9">
+        <v>21</v>
+      </c>
+      <c r="U35" s="9">
+        <v>27</v>
+      </c>
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
@@ -2915,7 +2983,7 @@
       <c r="AA35" s="9"/>
       <c r="AB35" s="9">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3278,8 +3346,12 @@
       </c>
       <c r="R43" s="9"/>
       <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
+      <c r="T43" s="9">
+        <v>26</v>
+      </c>
+      <c r="U43" s="9">
+        <v>33</v>
+      </c>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
       <c r="X43" s="9"/>
@@ -3288,7 +3360,7 @@
       <c r="AA43" s="9"/>
       <c r="AB43" s="9">
         <f t="shared" si="0"/>
-        <v>202</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3407,8 +3479,12 @@
       </c>
       <c r="R46" s="9"/>
       <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
+      <c r="T46" s="9">
+        <v>3</v>
+      </c>
+      <c r="U46" s="9">
+        <v>15</v>
+      </c>
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
       <c r="X46" s="9"/>
@@ -3417,7 +3493,7 @@
       <c r="AA46" s="9"/>
       <c r="AB46" s="9">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3462,8 +3538,12 @@
       </c>
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
+      <c r="T47" s="9">
+        <v>12</v>
+      </c>
+      <c r="U47" s="9">
+        <v>10</v>
+      </c>
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
       <c r="X47" s="9"/>
@@ -3472,7 +3552,7 @@
       <c r="AA47" s="9"/>
       <c r="AB47" s="9">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3562,8 +3642,12 @@
       </c>
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
+      <c r="T49" s="9">
+        <v>7</v>
+      </c>
+      <c r="U49" s="9">
+        <v>20</v>
+      </c>
       <c r="V49" s="9"/>
       <c r="W49" s="9"/>
       <c r="X49" s="9"/>
@@ -3572,7 +3656,7 @@
       <c r="AA49" s="9"/>
       <c r="AB49" s="9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3617,8 +3701,12 @@
       </c>
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
+      <c r="T50" s="9">
+        <v>8</v>
+      </c>
+      <c r="U50" s="9">
+        <v>15</v>
+      </c>
       <c r="V50" s="9"/>
       <c r="W50" s="9"/>
       <c r="X50" s="9"/>
@@ -3627,7 +3715,7 @@
       <c r="AA50" s="9"/>
       <c r="AB50" s="9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3672,8 +3760,12 @@
       </c>
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
+      <c r="T51" s="9">
+        <v>2</v>
+      </c>
+      <c r="U51" s="9">
+        <v>11</v>
+      </c>
       <c r="V51" s="9"/>
       <c r="W51" s="9"/>
       <c r="X51" s="9"/>
@@ -3682,7 +3774,7 @@
       <c r="AA51" s="9"/>
       <c r="AB51" s="9">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3952,8 +4044,12 @@
       </c>
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
-      <c r="T57" s="9"/>
-      <c r="U57" s="9"/>
+      <c r="T57" s="9">
+        <v>2</v>
+      </c>
+      <c r="U57" s="9">
+        <v>30</v>
+      </c>
       <c r="V57" s="9"/>
       <c r="W57" s="9"/>
       <c r="X57" s="9"/>
@@ -3962,7 +4058,7 @@
       <c r="AA57" s="9"/>
       <c r="AB57" s="9">
         <f t="shared" si="0"/>
-        <v>202</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4036,8 +4132,12 @@
       </c>
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
+      <c r="T59" s="9">
+        <v>16</v>
+      </c>
+      <c r="U59" s="9">
+        <v>8</v>
+      </c>
       <c r="V59" s="9"/>
       <c r="W59" s="9"/>
       <c r="X59" s="9"/>
@@ -4046,7 +4146,7 @@
       <c r="AA59" s="9"/>
       <c r="AB59" s="9">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4091,8 +4191,12 @@
       </c>
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
+      <c r="T60" s="9">
+        <v>10</v>
+      </c>
+      <c r="U60" s="9">
+        <v>12</v>
+      </c>
       <c r="V60" s="9"/>
       <c r="W60" s="9"/>
       <c r="X60" s="9"/>
@@ -4101,7 +4205,7 @@
       <c r="AA60" s="9"/>
       <c r="AB60" s="9">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4146,8 +4250,12 @@
       </c>
       <c r="R61" s="9"/>
       <c r="S61" s="9"/>
-      <c r="T61" s="9"/>
-      <c r="U61" s="9"/>
+      <c r="T61" s="9">
+        <v>7</v>
+      </c>
+      <c r="U61" s="9">
+        <v>13</v>
+      </c>
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
       <c r="X61" s="9"/>
@@ -4156,7 +4264,7 @@
       <c r="AA61" s="9"/>
       <c r="AB61" s="9">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4201,8 +4309,12 @@
       </c>
       <c r="R62" s="9"/>
       <c r="S62" s="9"/>
-      <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
+      <c r="T62" s="9">
+        <v>18</v>
+      </c>
+      <c r="U62" s="9">
+        <v>16</v>
+      </c>
       <c r="V62" s="9"/>
       <c r="W62" s="9"/>
       <c r="X62" s="9"/>
@@ -4211,7 +4323,7 @@
       <c r="AA62" s="9"/>
       <c r="AB62" s="9">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4256,8 +4368,12 @@
       </c>
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
-      <c r="T63" s="9"/>
-      <c r="U63" s="9"/>
+      <c r="T63" s="9">
+        <v>16</v>
+      </c>
+      <c r="U63" s="9">
+        <v>14</v>
+      </c>
       <c r="V63" s="9"/>
       <c r="W63" s="9"/>
       <c r="X63" s="9"/>
@@ -4266,7 +4382,7 @@
       <c r="AA63" s="9"/>
       <c r="AB63" s="9">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4581,8 +4697,12 @@
       </c>
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
-      <c r="T70" s="9"/>
-      <c r="U70" s="9"/>
+      <c r="T70" s="9">
+        <v>29</v>
+      </c>
+      <c r="U70" s="9">
+        <v>35</v>
+      </c>
       <c r="V70" s="9"/>
       <c r="W70" s="9"/>
       <c r="X70" s="9"/>
@@ -4591,7 +4711,7 @@
       <c r="AA70" s="9"/>
       <c r="AB70" s="9">
         <f t="shared" ref="AB70:AB133" si="1">SUM(J70:AA70)</f>
-        <v>199</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4665,8 +4785,12 @@
       </c>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
-      <c r="T72" s="9"/>
-      <c r="U72" s="9"/>
+      <c r="T72" s="9">
+        <v>24</v>
+      </c>
+      <c r="U72" s="9">
+        <v>7</v>
+      </c>
       <c r="V72" s="9"/>
       <c r="W72" s="9"/>
       <c r="X72" s="9"/>
@@ -4675,7 +4799,7 @@
       <c r="AA72" s="9"/>
       <c r="AB72" s="9">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4720,8 +4844,12 @@
       </c>
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
-      <c r="T73" s="9"/>
-      <c r="U73" s="9"/>
+      <c r="T73" s="9">
+        <v>18</v>
+      </c>
+      <c r="U73" s="9">
+        <v>0</v>
+      </c>
       <c r="V73" s="9"/>
       <c r="W73" s="9"/>
       <c r="X73" s="9"/>
@@ -4730,7 +4858,7 @@
       <c r="AA73" s="9"/>
       <c r="AB73" s="9">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4775,8 +4903,12 @@
       </c>
       <c r="R74" s="9"/>
       <c r="S74" s="9"/>
-      <c r="T74" s="9"/>
-      <c r="U74" s="9"/>
+      <c r="T74" s="9">
+        <v>21</v>
+      </c>
+      <c r="U74" s="9">
+        <v>3</v>
+      </c>
       <c r="V74" s="9"/>
       <c r="W74" s="9"/>
       <c r="X74" s="9"/>
@@ -4785,7 +4917,7 @@
       <c r="AA74" s="9"/>
       <c r="AB74" s="9">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4830,8 +4962,12 @@
       </c>
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
-      <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
+      <c r="T75" s="9">
+        <v>12</v>
+      </c>
+      <c r="U75" s="9">
+        <v>5</v>
+      </c>
       <c r="V75" s="9"/>
       <c r="W75" s="9"/>
       <c r="X75" s="9"/>
@@ -4840,7 +4976,7 @@
       <c r="AA75" s="9"/>
       <c r="AB75" s="9">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4885,8 +5021,12 @@
       </c>
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
-      <c r="T76" s="9"/>
-      <c r="U76" s="9"/>
+      <c r="T76" s="9">
+        <v>20</v>
+      </c>
+      <c r="U76" s="9">
+        <v>5</v>
+      </c>
       <c r="V76" s="9"/>
       <c r="W76" s="9"/>
       <c r="X76" s="9"/>
@@ -4895,7 +5035,7 @@
       <c r="AA76" s="9"/>
       <c r="AB76" s="9">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5210,8 +5350,12 @@
       </c>
       <c r="R83" s="9"/>
       <c r="S83" s="9"/>
-      <c r="T83" s="9"/>
-      <c r="U83" s="9"/>
+      <c r="T83" s="9">
+        <v>31</v>
+      </c>
+      <c r="U83" s="9">
+        <v>1</v>
+      </c>
       <c r="V83" s="9"/>
       <c r="W83" s="9"/>
       <c r="X83" s="9"/>
@@ -5220,7 +5364,7 @@
       <c r="AA83" s="9"/>
       <c r="AB83" s="9">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5294,8 +5438,12 @@
       </c>
       <c r="R85" s="9"/>
       <c r="S85" s="9"/>
-      <c r="T85" s="9"/>
-      <c r="U85" s="9"/>
+      <c r="T85" s="9">
+        <v>8</v>
+      </c>
+      <c r="U85" s="9">
+        <v>5</v>
+      </c>
       <c r="V85" s="9"/>
       <c r="W85" s="9"/>
       <c r="X85" s="9"/>
@@ -5304,7 +5452,7 @@
       <c r="AA85" s="9"/>
       <c r="AB85" s="9">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5402,8 +5550,12 @@
       </c>
       <c r="R87" s="9"/>
       <c r="S87" s="9"/>
-      <c r="T87" s="9"/>
-      <c r="U87" s="9"/>
+      <c r="T87" s="9">
+        <v>18</v>
+      </c>
+      <c r="U87" s="9">
+        <v>5</v>
+      </c>
       <c r="V87" s="9"/>
       <c r="W87" s="9"/>
       <c r="X87" s="9"/>
@@ -5412,7 +5564,7 @@
       <c r="AA87" s="9"/>
       <c r="AB87" s="9">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5512,8 +5664,12 @@
       </c>
       <c r="R89" s="9"/>
       <c r="S89" s="9"/>
-      <c r="T89" s="9"/>
-      <c r="U89" s="9"/>
+      <c r="T89" s="9">
+        <v>18</v>
+      </c>
+      <c r="U89" s="9">
+        <v>13</v>
+      </c>
       <c r="V89" s="9"/>
       <c r="W89" s="9"/>
       <c r="X89" s="9"/>
@@ -5522,7 +5678,7 @@
       <c r="AA89" s="9"/>
       <c r="AB89" s="9">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5606,8 +5762,12 @@
       </c>
       <c r="R91" s="9"/>
       <c r="S91" s="9"/>
-      <c r="T91" s="9"/>
-      <c r="U91" s="9"/>
+      <c r="T91" s="9">
+        <v>7</v>
+      </c>
+      <c r="U91" s="9">
+        <v>13</v>
+      </c>
       <c r="V91" s="9"/>
       <c r="W91" s="9"/>
       <c r="X91" s="9"/>
@@ -5616,7 +5776,7 @@
       <c r="AA91" s="9"/>
       <c r="AB91" s="9">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5696,8 +5856,12 @@
       <c r="Q93" s="9"/>
       <c r="R93" s="9"/>
       <c r="S93" s="9"/>
-      <c r="T93" s="9"/>
-      <c r="U93" s="9"/>
+      <c r="T93" s="9">
+        <v>15</v>
+      </c>
+      <c r="U93" s="9">
+        <v>10</v>
+      </c>
       <c r="V93" s="9"/>
       <c r="W93" s="9"/>
       <c r="X93" s="9"/>
@@ -5706,7 +5870,7 @@
       <c r="AA93" s="9"/>
       <c r="AB93" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5884,8 +6048,12 @@
       <c r="Q97" s="9"/>
       <c r="R97" s="9"/>
       <c r="S97" s="9"/>
-      <c r="T97" s="9"/>
-      <c r="U97" s="9"/>
+      <c r="T97" s="9">
+        <v>21</v>
+      </c>
+      <c r="U97" s="9">
+        <v>6</v>
+      </c>
       <c r="V97" s="9"/>
       <c r="W97" s="9"/>
       <c r="X97" s="9"/>
@@ -5894,7 +6062,7 @@
       <c r="AA97" s="9"/>
       <c r="AB97" s="9">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5968,8 +6136,12 @@
       </c>
       <c r="R99" s="9"/>
       <c r="S99" s="9"/>
-      <c r="T99" s="9"/>
-      <c r="U99" s="9"/>
+      <c r="T99" s="9">
+        <v>1</v>
+      </c>
+      <c r="U99" s="9">
+        <v>4</v>
+      </c>
       <c r="V99" s="9"/>
       <c r="W99" s="9"/>
       <c r="X99" s="9"/>
@@ -5978,7 +6150,7 @@
       <c r="AA99" s="9"/>
       <c r="AB99" s="9">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6023,8 +6195,12 @@
       </c>
       <c r="R100" s="9"/>
       <c r="S100" s="9"/>
-      <c r="T100" s="9"/>
-      <c r="U100" s="9"/>
+      <c r="T100" s="9">
+        <v>6</v>
+      </c>
+      <c r="U100" s="9">
+        <v>1</v>
+      </c>
       <c r="V100" s="9"/>
       <c r="W100" s="9"/>
       <c r="X100" s="9"/>
@@ -6033,7 +6209,7 @@
       <c r="AA100" s="9"/>
       <c r="AB100" s="9">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="101" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6078,8 +6254,12 @@
       </c>
       <c r="R101" s="9"/>
       <c r="S101" s="9"/>
-      <c r="T101" s="9"/>
-      <c r="U101" s="9"/>
+      <c r="T101" s="9">
+        <v>2</v>
+      </c>
+      <c r="U101" s="9">
+        <v>3</v>
+      </c>
       <c r="V101" s="9"/>
       <c r="W101" s="9"/>
       <c r="X101" s="9"/>
@@ -6088,7 +6268,7 @@
       <c r="AA101" s="9"/>
       <c r="AB101" s="9">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6133,8 +6313,12 @@
       </c>
       <c r="R102" s="9"/>
       <c r="S102" s="9"/>
-      <c r="T102" s="9"/>
-      <c r="U102" s="9"/>
+      <c r="T102" s="9">
+        <v>10</v>
+      </c>
+      <c r="U102" s="9">
+        <v>4</v>
+      </c>
       <c r="V102" s="9"/>
       <c r="W102" s="9"/>
       <c r="X102" s="9"/>
@@ -6143,7 +6327,7 @@
       <c r="AA102" s="9"/>
       <c r="AB102" s="9">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6188,8 +6372,12 @@
       </c>
       <c r="R103" s="9"/>
       <c r="S103" s="9"/>
-      <c r="T103" s="9"/>
-      <c r="U103" s="9"/>
+      <c r="T103" s="9">
+        <v>1</v>
+      </c>
+      <c r="U103" s="9">
+        <v>3</v>
+      </c>
       <c r="V103" s="9"/>
       <c r="W103" s="9"/>
       <c r="X103" s="9"/>
@@ -6198,7 +6386,7 @@
       <c r="AA103" s="9"/>
       <c r="AB103" s="9">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6513,8 +6701,12 @@
       </c>
       <c r="R110" s="9"/>
       <c r="S110" s="9"/>
-      <c r="T110" s="9"/>
-      <c r="U110" s="9"/>
+      <c r="T110" s="9">
+        <v>2</v>
+      </c>
+      <c r="U110" s="9">
+        <v>14</v>
+      </c>
       <c r="V110" s="9"/>
       <c r="W110" s="9"/>
       <c r="X110" s="9"/>
@@ -6523,7 +6715,7 @@
       <c r="AA110" s="9"/>
       <c r="AB110" s="9">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6597,8 +6789,12 @@
       </c>
       <c r="R112" s="9"/>
       <c r="S112" s="9"/>
-      <c r="T112" s="9"/>
-      <c r="U112" s="9"/>
+      <c r="T112" s="9">
+        <v>23</v>
+      </c>
+      <c r="U112" s="9">
+        <v>9</v>
+      </c>
       <c r="V112" s="9"/>
       <c r="W112" s="9"/>
       <c r="X112" s="9"/>
@@ -6607,7 +6803,7 @@
       <c r="AA112" s="9"/>
       <c r="AB112" s="9">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6652,8 +6848,12 @@
       </c>
       <c r="R113" s="9"/>
       <c r="S113" s="9"/>
-      <c r="T113" s="9"/>
-      <c r="U113" s="9"/>
+      <c r="T113" s="9">
+        <v>12</v>
+      </c>
+      <c r="U113" s="9">
+        <v>4</v>
+      </c>
       <c r="V113" s="9"/>
       <c r="W113" s="9"/>
       <c r="X113" s="9"/>
@@ -6662,7 +6862,7 @@
       <c r="AA113" s="9"/>
       <c r="AB113" s="9">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6707,8 +6907,12 @@
       </c>
       <c r="R114" s="9"/>
       <c r="S114" s="9"/>
-      <c r="T114" s="9"/>
-      <c r="U114" s="9"/>
+      <c r="T114" s="9">
+        <v>18</v>
+      </c>
+      <c r="U114" s="9">
+        <v>4</v>
+      </c>
       <c r="V114" s="9"/>
       <c r="W114" s="9"/>
       <c r="X114" s="9"/>
@@ -6717,7 +6921,7 @@
       <c r="AA114" s="9"/>
       <c r="AB114" s="9">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6762,8 +6966,12 @@
       </c>
       <c r="R115" s="9"/>
       <c r="S115" s="9"/>
-      <c r="T115" s="9"/>
-      <c r="U115" s="9"/>
+      <c r="T115" s="9">
+        <v>7</v>
+      </c>
+      <c r="U115" s="9">
+        <v>11</v>
+      </c>
       <c r="V115" s="9"/>
       <c r="W115" s="9"/>
       <c r="X115" s="9"/>
@@ -6772,7 +6980,7 @@
       <c r="AA115" s="9"/>
       <c r="AB115" s="9">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6817,8 +7025,12 @@
       </c>
       <c r="R116" s="9"/>
       <c r="S116" s="9"/>
-      <c r="T116" s="9"/>
-      <c r="U116" s="9"/>
+      <c r="T116" s="9">
+        <v>12</v>
+      </c>
+      <c r="U116" s="9">
+        <v>4</v>
+      </c>
       <c r="V116" s="9"/>
       <c r="W116" s="9"/>
       <c r="X116" s="9"/>
@@ -6827,7 +7039,7 @@
       <c r="AA116" s="9"/>
       <c r="AB116" s="9">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7142,8 +7354,12 @@
       </c>
       <c r="R123" s="9"/>
       <c r="S123" s="9"/>
-      <c r="T123" s="9"/>
-      <c r="U123" s="9"/>
+      <c r="T123" s="9">
+        <v>36</v>
+      </c>
+      <c r="U123" s="9">
+        <v>4</v>
+      </c>
       <c r="V123" s="9"/>
       <c r="W123" s="9"/>
       <c r="X123" s="9"/>
@@ -7152,7 +7368,7 @@
       <c r="AA123" s="9"/>
       <c r="AB123" s="9">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>248</v>
       </c>
     </row>
     <row r="124" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7226,8 +7442,12 @@
       </c>
       <c r="R125" s="9"/>
       <c r="S125" s="9"/>
-      <c r="T125" s="9"/>
-      <c r="U125" s="9"/>
+      <c r="T125" s="9">
+        <v>7</v>
+      </c>
+      <c r="U125" s="9">
+        <v>9</v>
+      </c>
       <c r="V125" s="9"/>
       <c r="W125" s="9"/>
       <c r="X125" s="9"/>
@@ -7236,7 +7456,7 @@
       <c r="AA125" s="9"/>
       <c r="AB125" s="9">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="126" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7328,8 +7548,12 @@
       </c>
       <c r="R127" s="9"/>
       <c r="S127" s="9"/>
-      <c r="T127" s="9"/>
-      <c r="U127" s="9"/>
+      <c r="T127" s="9">
+        <v>7</v>
+      </c>
+      <c r="U127" s="9">
+        <v>9</v>
+      </c>
       <c r="V127" s="9"/>
       <c r="W127" s="9"/>
       <c r="X127" s="9"/>
@@ -7338,7 +7562,7 @@
       <c r="AA127" s="9"/>
       <c r="AB127" s="9">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="128" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7428,8 +7652,12 @@
       </c>
       <c r="R129" s="9"/>
       <c r="S129" s="9"/>
-      <c r="T129" s="9"/>
-      <c r="U129" s="9"/>
+      <c r="T129" s="9">
+        <v>5</v>
+      </c>
+      <c r="U129" s="9">
+        <v>7</v>
+      </c>
       <c r="V129" s="9"/>
       <c r="W129" s="9"/>
       <c r="X129" s="9"/>
@@ -7438,7 +7666,7 @@
       <c r="AA129" s="9"/>
       <c r="AB129" s="9">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="130" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7484,7 +7712,9 @@
       <c r="R130" s="9"/>
       <c r="S130" s="9"/>
       <c r="T130" s="9"/>
-      <c r="U130" s="9"/>
+      <c r="U130" s="9">
+        <v>15</v>
+      </c>
       <c r="V130" s="9"/>
       <c r="W130" s="9"/>
       <c r="X130" s="9"/>
@@ -7493,7 +7723,7 @@
       <c r="AA130" s="9"/>
       <c r="AB130" s="9">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7628,8 +7858,12 @@
       </c>
       <c r="R133" s="9"/>
       <c r="S133" s="9"/>
-      <c r="T133" s="9"/>
-      <c r="U133" s="9"/>
+      <c r="T133" s="9">
+        <v>3</v>
+      </c>
+      <c r="U133" s="9">
+        <v>7</v>
+      </c>
       <c r="V133" s="9"/>
       <c r="W133" s="9"/>
       <c r="X133" s="9"/>
@@ -7638,7 +7872,7 @@
       <c r="AA133" s="9"/>
       <c r="AB133" s="9">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="134" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7763,7 +7997,9 @@
       <c r="Q136" s="9"/>
       <c r="R136" s="9"/>
       <c r="S136" s="9"/>
-      <c r="T136" s="9"/>
+      <c r="T136" s="9">
+        <v>1</v>
+      </c>
       <c r="U136" s="9"/>
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
@@ -7773,7 +8009,7 @@
       <c r="AA136" s="9"/>
       <c r="AB136" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7863,8 +8099,12 @@
       </c>
       <c r="R138" s="9"/>
       <c r="S138" s="9"/>
-      <c r="T138" s="9"/>
-      <c r="U138" s="9"/>
+      <c r="T138" s="9">
+        <v>9</v>
+      </c>
+      <c r="U138" s="9">
+        <v>-2</v>
+      </c>
       <c r="V138" s="9"/>
       <c r="W138" s="9"/>
       <c r="X138" s="9"/>
@@ -7873,7 +8113,7 @@
       <c r="AA138" s="9"/>
       <c r="AB138" s="9">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
añadida la semana 7
</commit_message>
<xml_diff>
--- a/LEC.xlsx
+++ b/LEC.xlsx
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:AC705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1433,15 +1433,19 @@
       <c r="U5" s="9">
         <v>16</v>
       </c>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
+      <c r="V5" s="9">
+        <v>1</v>
+      </c>
+      <c r="W5" s="9">
+        <v>15</v>
+      </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="9"/>
       <c r="AB5" s="9">
         <f>SUM(J5:AA5)</f>
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1492,15 +1496,19 @@
       <c r="U6" s="9">
         <v>23</v>
       </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
+      <c r="V6" s="9">
+        <v>4</v>
+      </c>
+      <c r="W6" s="9">
+        <v>6</v>
+      </c>
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9">
         <f t="shared" ref="AB6:AB69" si="0">SUM(J6:AA6)</f>
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1551,15 +1559,19 @@
       <c r="U7" s="9">
         <v>20</v>
       </c>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
+      <c r="V7" s="9">
+        <v>8</v>
+      </c>
+      <c r="W7" s="9">
+        <v>15</v>
+      </c>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="9">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1610,15 +1622,19 @@
       <c r="U8" s="9">
         <v>18</v>
       </c>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
+      <c r="V8" s="9">
+        <v>0</v>
+      </c>
+      <c r="W8" s="9">
+        <v>16</v>
+      </c>
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
       <c r="AB8" s="9">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1669,15 +1685,19 @@
       <c r="U9" s="9">
         <v>21</v>
       </c>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
+      <c r="V9" s="9">
+        <v>4</v>
+      </c>
+      <c r="W9" s="9">
+        <v>15</v>
+      </c>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
       <c r="AB9" s="9">
         <f t="shared" si="0"/>
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1998,15 +2018,19 @@
       <c r="U16" s="9">
         <v>31</v>
       </c>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
+      <c r="V16" s="9">
+        <v>11</v>
+      </c>
+      <c r="W16" s="9">
+        <v>25</v>
+      </c>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2086,15 +2110,19 @@
       <c r="U18" s="9">
         <v>10</v>
       </c>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
+      <c r="V18" s="9">
+        <v>14</v>
+      </c>
+      <c r="W18" s="9">
+        <v>7</v>
+      </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2145,15 +2173,19 @@
       <c r="U19" s="9">
         <v>8</v>
       </c>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
+      <c r="V19" s="9">
+        <v>14</v>
+      </c>
+      <c r="W19" s="9">
+        <v>8</v>
+      </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
       <c r="AA19" s="9"/>
       <c r="AB19" s="9">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2204,15 +2236,19 @@
       <c r="U20" s="9">
         <v>14</v>
       </c>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
+      <c r="V20" s="9">
+        <v>16</v>
+      </c>
+      <c r="W20" s="9">
+        <v>6</v>
+      </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AB20" s="9">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2263,15 +2299,19 @@
       <c r="U21" s="9">
         <v>27</v>
       </c>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
+      <c r="V21" s="9">
+        <v>30</v>
+      </c>
+      <c r="W21" s="9">
+        <v>9</v>
+      </c>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2322,15 +2362,19 @@
       <c r="U22" s="9">
         <v>21</v>
       </c>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
+      <c r="V22" s="9">
+        <v>15</v>
+      </c>
+      <c r="W22" s="9">
+        <v>4</v>
+      </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="9"/>
       <c r="AB22" s="9">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2651,15 +2695,19 @@
       <c r="U29" s="9">
         <v>34</v>
       </c>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
+      <c r="V29" s="9">
+        <v>31</v>
+      </c>
+      <c r="W29" s="9">
+        <v>12</v>
+      </c>
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9">
         <f t="shared" si="0"/>
-        <v>239</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2739,15 +2787,19 @@
       <c r="U31" s="9">
         <v>18</v>
       </c>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
+      <c r="V31" s="9">
+        <v>9</v>
+      </c>
+      <c r="W31" s="9">
+        <v>9</v>
+      </c>
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
       <c r="Z31" s="9"/>
       <c r="AA31" s="9"/>
       <c r="AB31" s="9">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2798,15 +2850,19 @@
       <c r="U32" s="9">
         <v>16</v>
       </c>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
+      <c r="V32" s="9">
+        <v>20</v>
+      </c>
+      <c r="W32" s="9">
+        <v>11</v>
+      </c>
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
       <c r="Z32" s="9"/>
       <c r="AA32" s="9"/>
       <c r="AB32" s="9">
         <f t="shared" si="0"/>
-        <v>161</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2857,15 +2913,19 @@
       <c r="U33" s="9">
         <v>22</v>
       </c>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
+      <c r="V33" s="9">
+        <v>25</v>
+      </c>
+      <c r="W33" s="9">
+        <v>22</v>
+      </c>
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
       <c r="AB33" s="9">
         <f t="shared" si="0"/>
-        <v>217</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2916,15 +2976,19 @@
       <c r="U34" s="9">
         <v>19</v>
       </c>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
+      <c r="V34" s="9">
+        <v>9</v>
+      </c>
+      <c r="W34" s="9">
+        <v>13</v>
+      </c>
       <c r="X34" s="9"/>
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
       <c r="AA34" s="9"/>
       <c r="AB34" s="9">
         <f t="shared" si="0"/>
-        <v>177</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2975,15 +3039,19 @@
       <c r="U35" s="9">
         <v>27</v>
       </c>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
+      <c r="V35" s="9">
+        <v>20</v>
+      </c>
+      <c r="W35" s="9">
+        <v>2</v>
+      </c>
       <c r="X35" s="9"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
       <c r="AA35" s="9"/>
       <c r="AB35" s="9">
         <f t="shared" si="0"/>
-        <v>188</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3352,15 +3420,19 @@
       <c r="U43" s="9">
         <v>33</v>
       </c>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
+      <c r="V43" s="9">
+        <v>33</v>
+      </c>
+      <c r="W43" s="9">
+        <v>25</v>
+      </c>
       <c r="X43" s="9"/>
       <c r="Y43" s="9"/>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9">
         <f t="shared" si="0"/>
-        <v>261</v>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3485,15 +3557,19 @@
       <c r="U46" s="9">
         <v>15</v>
       </c>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
+      <c r="V46" s="9">
+        <v>15</v>
+      </c>
+      <c r="W46" s="9">
+        <v>12</v>
+      </c>
       <c r="X46" s="9"/>
       <c r="Y46" s="9"/>
       <c r="Z46" s="9"/>
       <c r="AA46" s="9"/>
       <c r="AB46" s="9">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3544,15 +3620,19 @@
       <c r="U47" s="9">
         <v>10</v>
       </c>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
+      <c r="V47" s="9">
+        <v>15</v>
+      </c>
+      <c r="W47" s="9">
+        <v>3</v>
+      </c>
       <c r="X47" s="9"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="5:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3648,15 +3728,19 @@
       <c r="U49" s="9">
         <v>20</v>
       </c>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
+      <c r="V49" s="9">
+        <v>23</v>
+      </c>
+      <c r="W49" s="9">
+        <v>5</v>
+      </c>
       <c r="X49" s="9"/>
       <c r="Y49" s="9"/>
       <c r="Z49" s="9"/>
       <c r="AA49" s="9"/>
       <c r="AB49" s="9">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3707,15 +3791,19 @@
       <c r="U50" s="9">
         <v>15</v>
       </c>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
+      <c r="V50" s="9">
+        <v>14</v>
+      </c>
+      <c r="W50" s="9">
+        <v>7</v>
+      </c>
       <c r="X50" s="9"/>
       <c r="Y50" s="9"/>
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
       <c r="AB50" s="9">
         <f t="shared" si="0"/>
-        <v>148</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3766,15 +3854,19 @@
       <c r="U51" s="9">
         <v>11</v>
       </c>
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
+      <c r="V51" s="9">
+        <v>15</v>
+      </c>
+      <c r="W51" s="9">
+        <v>3</v>
+      </c>
       <c r="X51" s="9"/>
       <c r="Y51" s="9"/>
       <c r="Z51" s="9"/>
       <c r="AA51" s="9"/>
       <c r="AB51" s="9">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4050,15 +4142,19 @@
       <c r="U57" s="9">
         <v>30</v>
       </c>
-      <c r="V57" s="9"/>
-      <c r="W57" s="9"/>
+      <c r="V57" s="9">
+        <v>18</v>
+      </c>
+      <c r="W57" s="9">
+        <v>7</v>
+      </c>
       <c r="X57" s="9"/>
       <c r="Y57" s="9"/>
       <c r="Z57" s="9"/>
       <c r="AA57" s="9"/>
       <c r="AB57" s="9">
         <f t="shared" si="0"/>
-        <v>234</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4138,15 +4234,19 @@
       <c r="U59" s="9">
         <v>8</v>
       </c>
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
+      <c r="V59" s="9">
+        <v>10</v>
+      </c>
+      <c r="W59" s="9">
+        <v>15</v>
+      </c>
       <c r="X59" s="9"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="9"/>
       <c r="AA59" s="9"/>
       <c r="AB59" s="9">
         <f t="shared" si="0"/>
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4197,15 +4297,19 @@
       <c r="U60" s="9">
         <v>12</v>
       </c>
-      <c r="V60" s="9"/>
-      <c r="W60" s="9"/>
+      <c r="V60" s="9">
+        <v>11</v>
+      </c>
+      <c r="W60" s="9">
+        <v>12</v>
+      </c>
       <c r="X60" s="9"/>
       <c r="Y60" s="9"/>
       <c r="Z60" s="9"/>
       <c r="AA60" s="9"/>
       <c r="AB60" s="9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4256,15 +4360,19 @@
       <c r="U61" s="9">
         <v>13</v>
       </c>
-      <c r="V61" s="9"/>
-      <c r="W61" s="9"/>
+      <c r="V61" s="9">
+        <v>6</v>
+      </c>
+      <c r="W61" s="9">
+        <v>19</v>
+      </c>
       <c r="X61" s="9"/>
       <c r="Y61" s="9"/>
       <c r="Z61" s="9"/>
       <c r="AA61" s="9"/>
       <c r="AB61" s="9">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4315,15 +4423,19 @@
       <c r="U62" s="9">
         <v>16</v>
       </c>
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
+      <c r="V62" s="9">
+        <v>13</v>
+      </c>
+      <c r="W62" s="9">
+        <v>16</v>
+      </c>
       <c r="X62" s="9"/>
       <c r="Y62" s="9"/>
       <c r="Z62" s="9"/>
       <c r="AA62" s="9"/>
       <c r="AB62" s="9">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4374,15 +4486,19 @@
       <c r="U63" s="9">
         <v>14</v>
       </c>
-      <c r="V63" s="9"/>
-      <c r="W63" s="9"/>
+      <c r="V63" s="9">
+        <v>6</v>
+      </c>
+      <c r="W63" s="9">
+        <v>9</v>
+      </c>
       <c r="X63" s="9"/>
       <c r="Y63" s="9"/>
       <c r="Z63" s="9"/>
       <c r="AA63" s="9"/>
       <c r="AB63" s="9">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4703,15 +4819,19 @@
       <c r="U70" s="9">
         <v>35</v>
       </c>
-      <c r="V70" s="9"/>
-      <c r="W70" s="9"/>
+      <c r="V70" s="9">
+        <v>5</v>
+      </c>
+      <c r="W70" s="9">
+        <v>24</v>
+      </c>
       <c r="X70" s="9"/>
       <c r="Y70" s="9"/>
       <c r="Z70" s="9"/>
       <c r="AA70" s="9"/>
       <c r="AB70" s="9">
         <f t="shared" ref="AB70:AB133" si="1">SUM(J70:AA70)</f>
-        <v>263</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4791,15 +4911,19 @@
       <c r="U72" s="9">
         <v>7</v>
       </c>
-      <c r="V72" s="9"/>
-      <c r="W72" s="9"/>
+      <c r="V72" s="9">
+        <v>6</v>
+      </c>
+      <c r="W72" s="9">
+        <v>22</v>
+      </c>
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
       <c r="AB72" s="9">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4850,15 +4974,19 @@
       <c r="U73" s="9">
         <v>0</v>
       </c>
-      <c r="V73" s="9"/>
-      <c r="W73" s="9"/>
+      <c r="V73" s="9">
+        <v>12</v>
+      </c>
+      <c r="W73" s="9">
+        <v>21</v>
+      </c>
       <c r="X73" s="9"/>
       <c r="Y73" s="9"/>
       <c r="Z73" s="9"/>
       <c r="AA73" s="9"/>
       <c r="AB73" s="9">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4909,15 +5037,19 @@
       <c r="U74" s="9">
         <v>3</v>
       </c>
-      <c r="V74" s="9"/>
-      <c r="W74" s="9"/>
+      <c r="V74" s="9">
+        <v>22</v>
+      </c>
+      <c r="W74" s="9">
+        <v>28</v>
+      </c>
       <c r="X74" s="9"/>
       <c r="Y74" s="9"/>
       <c r="Z74" s="9"/>
       <c r="AA74" s="9"/>
       <c r="AB74" s="9">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4968,15 +5100,19 @@
       <c r="U75" s="9">
         <v>5</v>
       </c>
-      <c r="V75" s="9"/>
-      <c r="W75" s="9"/>
+      <c r="V75" s="9">
+        <v>20</v>
+      </c>
+      <c r="W75" s="9">
+        <v>27</v>
+      </c>
       <c r="X75" s="9"/>
       <c r="Y75" s="9"/>
       <c r="Z75" s="9"/>
       <c r="AA75" s="9"/>
       <c r="AB75" s="9">
         <f t="shared" si="1"/>
-        <v>127</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5027,15 +5163,19 @@
       <c r="U76" s="9">
         <v>5</v>
       </c>
-      <c r="V76" s="9"/>
-      <c r="W76" s="9"/>
+      <c r="V76" s="9">
+        <v>23</v>
+      </c>
+      <c r="W76" s="9">
+        <v>24</v>
+      </c>
       <c r="X76" s="9"/>
       <c r="Y76" s="9"/>
       <c r="Z76" s="9"/>
       <c r="AA76" s="9"/>
       <c r="AB76" s="9">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5356,15 +5496,19 @@
       <c r="U83" s="9">
         <v>1</v>
       </c>
-      <c r="V83" s="9"/>
-      <c r="W83" s="9"/>
+      <c r="V83" s="9">
+        <v>32</v>
+      </c>
+      <c r="W83" s="9">
+        <v>31</v>
+      </c>
       <c r="X83" s="9"/>
       <c r="Y83" s="9"/>
       <c r="Z83" s="9"/>
       <c r="AA83" s="9"/>
       <c r="AB83" s="9">
         <f t="shared" si="1"/>
-        <v>231</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5444,15 +5588,19 @@
       <c r="U85" s="9">
         <v>5</v>
       </c>
-      <c r="V85" s="9"/>
-      <c r="W85" s="9"/>
+      <c r="V85" s="9">
+        <v>13</v>
+      </c>
+      <c r="W85" s="9">
+        <v>12</v>
+      </c>
       <c r="X85" s="9"/>
       <c r="Y85" s="9"/>
       <c r="Z85" s="9"/>
       <c r="AA85" s="9"/>
       <c r="AB85" s="9">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5556,15 +5704,19 @@
       <c r="U87" s="9">
         <v>5</v>
       </c>
-      <c r="V87" s="9"/>
-      <c r="W87" s="9"/>
+      <c r="V87" s="9">
+        <v>9</v>
+      </c>
+      <c r="W87" s="9">
+        <v>22</v>
+      </c>
       <c r="X87" s="9"/>
       <c r="Y87" s="9"/>
       <c r="Z87" s="9"/>
       <c r="AA87" s="9"/>
       <c r="AB87" s="9">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5670,15 +5822,19 @@
       <c r="U89" s="9">
         <v>13</v>
       </c>
-      <c r="V89" s="9"/>
-      <c r="W89" s="9"/>
+      <c r="V89" s="9">
+        <v>4</v>
+      </c>
+      <c r="W89" s="9">
+        <v>12</v>
+      </c>
       <c r="X89" s="9"/>
       <c r="Y89" s="9"/>
       <c r="Z89" s="9"/>
       <c r="AA89" s="9"/>
       <c r="AB89" s="9">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5768,15 +5924,19 @@
       <c r="U91" s="9">
         <v>13</v>
       </c>
-      <c r="V91" s="9"/>
-      <c r="W91" s="9"/>
+      <c r="V91" s="9">
+        <v>4</v>
+      </c>
+      <c r="W91" s="9">
+        <v>25</v>
+      </c>
       <c r="X91" s="9"/>
       <c r="Y91" s="9"/>
       <c r="Z91" s="9"/>
       <c r="AA91" s="9"/>
       <c r="AB91" s="9">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5862,15 +6022,19 @@
       <c r="U93" s="9">
         <v>10</v>
       </c>
-      <c r="V93" s="9"/>
-      <c r="W93" s="9"/>
+      <c r="V93" s="9">
+        <v>16</v>
+      </c>
+      <c r="W93" s="9">
+        <v>22</v>
+      </c>
       <c r="X93" s="9"/>
       <c r="Y93" s="9"/>
       <c r="Z93" s="9"/>
       <c r="AA93" s="9"/>
       <c r="AB93" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6054,15 +6218,19 @@
       <c r="U97" s="9">
         <v>6</v>
       </c>
-      <c r="V97" s="9"/>
-      <c r="W97" s="9"/>
+      <c r="V97" s="9">
+        <v>12</v>
+      </c>
+      <c r="W97" s="9">
+        <v>28</v>
+      </c>
       <c r="X97" s="9"/>
       <c r="Y97" s="9"/>
       <c r="Z97" s="9"/>
       <c r="AA97" s="9"/>
       <c r="AB97" s="9">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6142,15 +6310,19 @@
       <c r="U99" s="9">
         <v>4</v>
       </c>
-      <c r="V99" s="9"/>
-      <c r="W99" s="9"/>
+      <c r="V99" s="9">
+        <v>6</v>
+      </c>
+      <c r="W99" s="9">
+        <v>13</v>
+      </c>
       <c r="X99" s="9"/>
       <c r="Y99" s="9"/>
       <c r="Z99" s="9"/>
       <c r="AA99" s="9"/>
       <c r="AB99" s="9">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6201,15 +6373,19 @@
       <c r="U100" s="9">
         <v>1</v>
       </c>
-      <c r="V100" s="9"/>
-      <c r="W100" s="9"/>
+      <c r="V100" s="9">
+        <v>2</v>
+      </c>
+      <c r="W100" s="9">
+        <v>7</v>
+      </c>
       <c r="X100" s="9"/>
       <c r="Y100" s="9"/>
       <c r="Z100" s="9"/>
       <c r="AA100" s="9"/>
       <c r="AB100" s="9">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6260,15 +6436,19 @@
       <c r="U101" s="9">
         <v>3</v>
       </c>
-      <c r="V101" s="9"/>
-      <c r="W101" s="9"/>
+      <c r="V101" s="9">
+        <v>8</v>
+      </c>
+      <c r="W101" s="9">
+        <v>12</v>
+      </c>
       <c r="X101" s="9"/>
       <c r="Y101" s="9"/>
       <c r="Z101" s="9"/>
       <c r="AA101" s="9"/>
       <c r="AB101" s="9">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6319,15 +6499,19 @@
       <c r="U102" s="9">
         <v>4</v>
       </c>
-      <c r="V102" s="9"/>
-      <c r="W102" s="9"/>
+      <c r="V102" s="9">
+        <v>4</v>
+      </c>
+      <c r="W102" s="9">
+        <v>14</v>
+      </c>
       <c r="X102" s="9"/>
       <c r="Y102" s="9"/>
       <c r="Z102" s="9"/>
       <c r="AA102" s="9"/>
       <c r="AB102" s="9">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6378,15 +6562,19 @@
       <c r="U103" s="9">
         <v>3</v>
       </c>
-      <c r="V103" s="9"/>
-      <c r="W103" s="9"/>
+      <c r="V103" s="9">
+        <v>4</v>
+      </c>
+      <c r="W103" s="9">
+        <v>7</v>
+      </c>
       <c r="X103" s="9"/>
       <c r="Y103" s="9"/>
       <c r="Z103" s="9"/>
       <c r="AA103" s="9"/>
       <c r="AB103" s="9">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="104" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6707,15 +6895,19 @@
       <c r="U110" s="9">
         <v>14</v>
       </c>
-      <c r="V110" s="9"/>
-      <c r="W110" s="9"/>
+      <c r="V110" s="9">
+        <v>14</v>
+      </c>
+      <c r="W110" s="9">
+        <v>5</v>
+      </c>
       <c r="X110" s="9"/>
       <c r="Y110" s="9"/>
       <c r="Z110" s="9"/>
       <c r="AA110" s="9"/>
       <c r="AB110" s="9">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6795,15 +6987,19 @@
       <c r="U112" s="9">
         <v>9</v>
       </c>
-      <c r="V112" s="9"/>
-      <c r="W112" s="9"/>
+      <c r="V112" s="9">
+        <v>14</v>
+      </c>
+      <c r="W112" s="9">
+        <v>3</v>
+      </c>
       <c r="X112" s="9"/>
       <c r="Y112" s="9"/>
       <c r="Z112" s="9"/>
       <c r="AA112" s="9"/>
       <c r="AB112" s="9">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6854,15 +7050,19 @@
       <c r="U113" s="9">
         <v>4</v>
       </c>
-      <c r="V113" s="9"/>
-      <c r="W113" s="9"/>
+      <c r="V113" s="9">
+        <v>18</v>
+      </c>
+      <c r="W113" s="9">
+        <v>2</v>
+      </c>
       <c r="X113" s="9"/>
       <c r="Y113" s="9"/>
       <c r="Z113" s="9"/>
       <c r="AA113" s="9"/>
       <c r="AB113" s="9">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6913,15 +7113,19 @@
       <c r="U114" s="9">
         <v>4</v>
       </c>
-      <c r="V114" s="9"/>
-      <c r="W114" s="9"/>
+      <c r="V114" s="9">
+        <v>20</v>
+      </c>
+      <c r="W114" s="9">
+        <v>-4</v>
+      </c>
       <c r="X114" s="9"/>
       <c r="Y114" s="9"/>
       <c r="Z114" s="9"/>
       <c r="AA114" s="9"/>
       <c r="AB114" s="9">
         <f t="shared" si="1"/>
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6972,15 +7176,19 @@
       <c r="U115" s="9">
         <v>11</v>
       </c>
-      <c r="V115" s="9"/>
-      <c r="W115" s="9"/>
+      <c r="V115" s="9">
+        <v>16</v>
+      </c>
+      <c r="W115" s="9">
+        <v>-5</v>
+      </c>
       <c r="X115" s="9"/>
       <c r="Y115" s="9"/>
       <c r="Z115" s="9"/>
       <c r="AA115" s="9"/>
       <c r="AB115" s="9">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7031,15 +7239,19 @@
       <c r="U116" s="9">
         <v>4</v>
       </c>
-      <c r="V116" s="9"/>
-      <c r="W116" s="9"/>
+      <c r="V116" s="9">
+        <v>20</v>
+      </c>
+      <c r="W116" s="9">
+        <v>0</v>
+      </c>
       <c r="X116" s="9"/>
       <c r="Y116" s="9"/>
       <c r="Z116" s="9"/>
       <c r="AA116" s="9"/>
       <c r="AB116" s="9">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7360,7 +7572,9 @@
       <c r="U123" s="9">
         <v>4</v>
       </c>
-      <c r="V123" s="9"/>
+      <c r="V123" s="9">
+        <v>44</v>
+      </c>
       <c r="W123" s="9"/>
       <c r="X123" s="9"/>
       <c r="Y123" s="9"/>
@@ -7368,7 +7582,7 @@
       <c r="AA123" s="9"/>
       <c r="AB123" s="9">
         <f t="shared" si="1"/>
-        <v>248</v>
+        <v>292</v>
       </c>
     </row>
     <row r="124" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7448,15 +7662,19 @@
       <c r="U125" s="9">
         <v>9</v>
       </c>
-      <c r="V125" s="9"/>
-      <c r="W125" s="9"/>
+      <c r="V125" s="9">
+        <v>4</v>
+      </c>
+      <c r="W125" s="9">
+        <v>5</v>
+      </c>
       <c r="X125" s="9"/>
       <c r="Y125" s="9"/>
       <c r="Z125" s="9"/>
       <c r="AA125" s="9"/>
       <c r="AB125" s="9">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7554,15 +7772,19 @@
       <c r="U127" s="9">
         <v>9</v>
       </c>
-      <c r="V127" s="9"/>
-      <c r="W127" s="9"/>
+      <c r="V127" s="9">
+        <v>3</v>
+      </c>
+      <c r="W127" s="9">
+        <v>12</v>
+      </c>
       <c r="X127" s="9"/>
       <c r="Y127" s="9"/>
       <c r="Z127" s="9"/>
       <c r="AA127" s="9"/>
       <c r="AB127" s="9">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="128" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7599,15 +7821,19 @@
       <c r="S128" s="9"/>
       <c r="T128" s="9"/>
       <c r="U128" s="9"/>
-      <c r="V128" s="9"/>
-      <c r="W128" s="9"/>
+      <c r="V128" s="9">
+        <v>-4</v>
+      </c>
+      <c r="W128" s="9">
+        <v>16</v>
+      </c>
       <c r="X128" s="9"/>
       <c r="Y128" s="9"/>
       <c r="Z128" s="9"/>
       <c r="AA128" s="9"/>
       <c r="AB128" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7658,15 +7884,19 @@
       <c r="U129" s="9">
         <v>7</v>
       </c>
-      <c r="V129" s="9"/>
-      <c r="W129" s="9"/>
+      <c r="V129" s="9">
+        <v>-1</v>
+      </c>
+      <c r="W129" s="9">
+        <v>13</v>
+      </c>
       <c r="X129" s="9"/>
       <c r="Y129" s="9"/>
       <c r="Z129" s="9"/>
       <c r="AA129" s="9"/>
       <c r="AB129" s="9">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8001,15 +8231,19 @@
         <v>1</v>
       </c>
       <c r="U136" s="9"/>
-      <c r="V136" s="9"/>
-      <c r="W136" s="9"/>
+      <c r="V136" s="9">
+        <v>2</v>
+      </c>
+      <c r="W136" s="9">
+        <v>11</v>
+      </c>
       <c r="X136" s="9"/>
       <c r="Y136" s="9"/>
       <c r="Z136" s="9"/>
       <c r="AA136" s="9"/>
       <c r="AB136" s="9">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8105,15 +8339,19 @@
       <c r="U138" s="9">
         <v>-2</v>
       </c>
-      <c r="V138" s="9"/>
-      <c r="W138" s="9"/>
+      <c r="V138" s="9">
+        <v>1</v>
+      </c>
+      <c r="W138" s="9">
+        <v>13</v>
+      </c>
       <c r="X138" s="9"/>
       <c r="Y138" s="9"/>
       <c r="Z138" s="9"/>
       <c r="AA138" s="9"/>
       <c r="AB138" s="9">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="5:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>